<commit_message>
Went through and inspected fits closely, most good a couple bad. Changed a few variables/functions. Excel sheet updated with closely inspected comments.
</commit_message>
<xml_diff>
--- a/OrderInfo.xlsx
+++ b/OrderInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmk2347/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmk2347/codes/coudereduction/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Order #</t>
   </si>
@@ -56,16 +56,7 @@
     <t>Range</t>
   </si>
   <si>
-    <t>Weird. Looks fine but can't get below 1 km/s?</t>
-  </si>
-  <si>
     <t>Dist From Last</t>
-  </si>
-  <si>
-    <t>BAD? Points &gt; 1km/s but no rejects</t>
-  </si>
-  <si>
-    <t>Def Bad</t>
   </si>
   <si>
     <t>Def REALLY Bad</t>
@@ -74,10 +65,61 @@
     <t>I don’t think THAT bad</t>
   </si>
   <si>
-    <t>I don’t think THAT bad, but worse at end?</t>
+    <t>Nothing at all really bad</t>
   </si>
   <si>
-    <t>Nothing at all really bad</t>
+    <t>Fit looks good</t>
+  </si>
+  <si>
+    <t>Peaks SNR</t>
+  </si>
+  <si>
+    <t>Fit is okay. Going to SNR=5 got us to 10 peaks but really didn't improve the fit</t>
+  </si>
+  <si>
+    <t>Fit is fine. Goint to SNR=20 got us 14 peaks, but not an extreme improvement</t>
+  </si>
+  <si>
+    <t>Not a bad fit. SNR=20:peaks=14, only slightly better?</t>
+  </si>
+  <si>
+    <t>Not a bad fit. SNR=20:peaks=15, only slightly better?</t>
+  </si>
+  <si>
+    <t>So can't get below 1 km/s while rejecting at 3mad, but the fit doesn't look horrific, just not perfect.</t>
+  </si>
+  <si>
+    <t>Fit is fine. SNR=20:peaks=13, but not much better</t>
+  </si>
+  <si>
+    <t>Was BAD with SNR=50, GOOD with SNR=20</t>
+  </si>
+  <si>
+    <t>Was BAD with SNR=50, GOOD with SNR=5</t>
+  </si>
+  <si>
+    <t>BAD with SNR=50. With SNR=20, fit looks good but wavkeeps look weird?</t>
+  </si>
+  <si>
+    <t>Fit isn't great. But can't really get better with lower SNR</t>
+  </si>
+  <si>
+    <t>Fit is fine.</t>
+  </si>
+  <si>
+    <t>SNR=50 wasn't bad, SNR=5 is a bit better</t>
+  </si>
+  <si>
+    <t>Bad with SNR=50, good with SNR=5</t>
+  </si>
+  <si>
+    <t>Bad at end with SNR=50, better with SNR=20</t>
+  </si>
+  <si>
+    <t>Might not be great at end, but really no lines there to help out</t>
+  </si>
+  <si>
+    <t>Spec Order</t>
   </si>
 </sst>
 </file>
@@ -93,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,7 +144,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -119,15 +167,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +475,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$48</c:f>
+              <c:f>Sheet1!$I$3:$I$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="46"/>
@@ -505,19 +561,19 @@
                   <c:v>11.39999999999964</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>15.5</c:v>
+                  <c:v>13.80000000000018</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>17.30000000000018</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15.69999999999982</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>21.19999999999982</c:v>
+                  <c:v>21.90000000000055</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>27.80000000000018</c:v>
+                  <c:v>27.30000000000018</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>29.0</c:v>
@@ -538,28 +594,28 @@
                   <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>56.5</c:v>
+                  <c:v>56.69999999999981</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>84.5</c:v>
+                  <c:v>61.39999999999964</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>68.0</c:v>
+                  <c:v>69.1999999999989</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>76.70000000000073</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>78.79999999999927</c:v>
+                  <c:v>82.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>97.10000000000036</c:v>
+                  <c:v>92.89999999999963</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>102.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>115.7999999999993</c:v>
+                  <c:v>113.3999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -574,11 +630,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1911337280"/>
-        <c:axId val="1897566464"/>
+        <c:axId val="-975726480"/>
+        <c:axId val="-975721680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1911337280"/>
+        <c:axId val="-975726480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,12 +691,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1897566464"/>
+        <c:crossAx val="-975721680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1897566464"/>
+        <c:axId val="-975721680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -698,7 +754,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1911337280"/>
+        <c:crossAx val="-975726480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -861,7 +917,93 @@
             <c:trendlineType val="poly"/>
             <c:order val="4"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.114608263446462"/>
+                  <c:y val="0.636131906140684"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 7E-06x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="30000"/>
+                      <a:t>4</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t> - 0.0004x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="30000"/>
+                      <a:t>3</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t> + 0.0185x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t> + 0.5793x + 61.973</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1015,7 +1157,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$48</c:f>
+              <c:f>Sheet1!$G$2:$G$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="47"/>
@@ -1104,16 +1246,16 @@
                   <c:v>105.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>105.8000000000002</c:v>
+                  <c:v>107.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>108.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>114.3999999999996</c:v>
+                  <c:v>111.5999999999995</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>112.9000000000005</c:v>
+                  <c:v>112.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>116.0</c:v>
@@ -1137,10 +1279,10 @@
                   <c:v>132.1000000000004</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>113.6000000000004</c:v>
+                  <c:v>136.500000000001</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>139.7999999999993</c:v>
+                  <c:v>138.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>142.0</c:v>
@@ -1149,13 +1291,13 @@
                   <c:v>147.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>148.7999999999993</c:v>
+                  <c:v>149.2999999999993</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>153.3999999999996</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>154.7000000000007</c:v>
+                  <c:v>157.1000000000004</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>161.2000000000007</c:v>
@@ -1173,11 +1315,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1916638000"/>
-        <c:axId val="1915981776"/>
+        <c:axId val="-975691744"/>
+        <c:axId val="-975686944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1916638000"/>
+        <c:axId val="-975691744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1233,12 +1375,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1915981776"/>
+        <c:crossAx val="-975686944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1915981776"/>
+        <c:axId val="-975686944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60.0"/>
@@ -1295,7 +1437,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1916638000"/>
+        <c:crossAx val="-975691744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1466,7 +1608,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$48</c:f>
+              <c:f>Sheet1!$F$3:$F$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="46"/>
@@ -1552,16 +1694,16 @@
                   <c:v>6366.05</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6487.1</c:v>
+                  <c:v>6486.15</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>6611.450000000001</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6738.5</c:v>
+                  <c:v>6740.4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6873.35</c:v>
+                  <c:v>6874.200000000001</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>7015.6</c:v>
@@ -1585,10 +1727,10 @@
                   <c:v>7994.45</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>8173.8</c:v>
+                  <c:v>8185.450000000001</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8385.0</c:v>
+                  <c:v>8384.400000000001</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>8593.9</c:v>
@@ -1597,13 +1739,13 @@
                   <c:v>8815.400000000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>9042.4</c:v>
+                  <c:v>9046.35</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>9290.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>9547.25</c:v>
+                  <c:v>9548.450000000001</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>9821.0</c:v>
@@ -1613,7 +1755,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$48</c:f>
+              <c:f>Sheet1!$I$3:$I$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="46"/>
@@ -1699,19 +1841,19 @@
                   <c:v>11.39999999999964</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>15.5</c:v>
+                  <c:v>13.80000000000018</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>17.30000000000018</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15.69999999999982</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>21.19999999999982</c:v>
+                  <c:v>21.90000000000055</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>27.80000000000018</c:v>
+                  <c:v>27.30000000000018</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>29.0</c:v>
@@ -1732,28 +1874,28 @@
                   <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>56.5</c:v>
+                  <c:v>56.69999999999981</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>84.5</c:v>
+                  <c:v>61.39999999999964</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>68.0</c:v>
+                  <c:v>69.1999999999989</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>76.70000000000073</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>78.79999999999927</c:v>
+                  <c:v>82.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>97.10000000000036</c:v>
+                  <c:v>92.89999999999963</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>102.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>115.7999999999993</c:v>
+                  <c:v>113.3999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1768,11 +1910,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1910114000"/>
-        <c:axId val="1909484656"/>
+        <c:axId val="-975626272"/>
+        <c:axId val="-975621472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1910114000"/>
+        <c:axId val="-975626272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1828,12 +1970,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1909484656"/>
+        <c:crossAx val="-975621472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1909484656"/>
+        <c:axId val="-975621472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -1892,7 +2034,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1910114000"/>
+        <c:crossAx val="-975626272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3613,13 +3755,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
@@ -3643,13 +3785,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
@@ -3673,13 +3815,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>698500</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>622300</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
@@ -3967,27 +4109,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="38.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="46.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3995,1580 +4138,2172 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>11</v>
       </c>
       <c r="B2" s="1">
-        <f>A2-11</f>
+        <f t="shared" ref="B2:B49" si="0">A2-11</f>
         <v>0</v>
       </c>
       <c r="C2" s="1">
+        <f>F3/(F3-F2)</f>
+        <v>80.920903954801702</v>
+      </c>
+      <c r="D2" s="1">
         <v>4208.7</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>4278.8999999999996</v>
       </c>
-      <c r="E2" s="1">
-        <f t="shared" ref="E2:E33" si="0">(D2+C2)/2</f>
+      <c r="F2" s="1">
+        <f t="shared" ref="F2:F33" si="1">(E2+D2)/2</f>
         <v>4243.7999999999993</v>
       </c>
-      <c r="F2" s="1">
-        <f>D2-C2</f>
+      <c r="G2" s="1">
+        <f>E2-D2</f>
         <v>70.199999999999818</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>10</v>
       </c>
+      <c r="J2" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>12</v>
       </c>
       <c r="B3" s="1">
-        <f>A3-11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C3" s="1">
+        <f t="shared" ref="C3:C49" si="2">F4/(F4-F3)</f>
+        <v>79.987132352940378</v>
+      </c>
+      <c r="D3" s="1">
         <v>4261.3</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>4332.5</v>
       </c>
-      <c r="E3" s="1">
-        <f t="shared" si="0"/>
+      <c r="F3" s="1">
+        <f t="shared" si="1"/>
         <v>4296.8999999999996</v>
       </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F49" si="1">D3-C3</f>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G49" si="3">E3-D3</f>
         <v>71.199999999999818</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>10</v>
       </c>
-      <c r="H3">
-        <f>C3-D2</f>
+      <c r="I3" s="1">
+        <f>D3-E2</f>
         <v>-17.599999999999454</v>
       </c>
+      <c r="J3" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>13</v>
       </c>
       <c r="B4" s="1">
-        <f>A4-11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C4" s="1">
+        <f t="shared" si="2"/>
+        <v>78.980286738350998</v>
+      </c>
+      <c r="D4" s="1">
         <v>4315.3</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>4387.3</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>4351.3</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="1"/>
+        <v>4351.3</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>17</v>
       </c>
-      <c r="H4">
-        <f t="shared" ref="H4:H49" si="2">C4-D3</f>
+      <c r="I4" s="1">
+        <f t="shared" ref="I4:I49" si="4">D4-E3</f>
         <v>-17.199999999999818</v>
       </c>
+      <c r="J4" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>14</v>
       </c>
       <c r="B5" s="1">
-        <f>A5-11</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C5" s="1">
+        <f t="shared" si="2"/>
+        <v>77.979912663755471</v>
+      </c>
+      <c r="D5" s="1">
         <v>4370.6000000000004</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>4443.6000000000004</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>4407.1000000000004</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="1"/>
+        <v>4407.1000000000004</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>9</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="2"/>
+      <c r="I5" s="1">
+        <f t="shared" si="4"/>
         <v>-16.699999999999818</v>
       </c>
+      <c r="J5" s="1">
+        <v>50</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>15</v>
       </c>
       <c r="B6" s="1">
-        <f>A6-11</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C6" s="1">
+        <f t="shared" si="2"/>
+        <v>76.924319727892097</v>
+      </c>
+      <c r="D6" s="1">
         <v>4427.3999999999996</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>4501.3</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>4464.3500000000004</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
+        <v>4464.3500000000004</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="3"/>
         <v>73.900000000000546</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>12</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="2"/>
+      <c r="I6" s="1">
+        <f t="shared" si="4"/>
         <v>-16.200000000000728</v>
       </c>
+      <c r="J6" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>16</v>
       </c>
       <c r="B7" s="1">
-        <f>A7-11</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C7" s="1">
+        <f t="shared" si="2"/>
+        <v>76.010779436152333</v>
+      </c>
+      <c r="D7" s="1">
         <v>4485.7</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>4560.6000000000004</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>4523.1499999999996</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="1"/>
+        <v>4523.1499999999996</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="3"/>
         <v>74.900000000000546</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>11</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="2"/>
+      <c r="I7" s="1">
+        <f t="shared" si="4"/>
         <v>-15.600000000000364</v>
       </c>
+      <c r="J7" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>17</v>
       </c>
       <c r="B8" s="1">
-        <f>A8-11</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C8" s="1">
+        <f t="shared" si="2"/>
+        <v>74.926612903225802</v>
+      </c>
+      <c r="D8" s="1">
         <v>4545.5</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>4621.3999999999996</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>4583.45</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="1"/>
+        <v>4583.45</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="3"/>
         <v>75.899999999999636</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>12</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="2"/>
+      <c r="I8" s="1">
+        <f t="shared" si="4"/>
         <v>-15.100000000000364</v>
       </c>
+      <c r="J8" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>18</v>
       </c>
       <c r="B9" s="1">
-        <f>A9-11</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C9" s="1">
+        <f t="shared" si="2"/>
+        <v>74.041666666666245</v>
+      </c>
+      <c r="D9" s="1">
         <v>4607</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>4683.8999999999996</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>4645.45</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="1"/>
+        <v>4645.45</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="3"/>
         <v>76.899999999999636</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>7</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
+      <c r="I9" s="1">
+        <f t="shared" si="4"/>
         <v>-14.399999999999636</v>
       </c>
+      <c r="J9" s="1">
+        <v>50</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>19</v>
       </c>
       <c r="B10" s="1">
-        <f>A10-11</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C10" s="1">
+        <f t="shared" si="2"/>
+        <v>72.948815889992559</v>
+      </c>
+      <c r="D10" s="1">
         <v>4670.1000000000004</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>4748</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>4709.05</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="1"/>
+        <v>4709.05</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="3"/>
         <v>77.899999999999636</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>13</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
+      <c r="I10" s="1">
+        <f t="shared" si="4"/>
         <v>-13.799999999999272</v>
       </c>
+      <c r="J10" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>20</v>
       </c>
       <c r="B11" s="1">
-        <f>A11-11</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C11" s="1">
+        <f t="shared" si="2"/>
+        <v>71.996282527881036</v>
+      </c>
+      <c r="D11" s="1">
         <v>4735</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>4814</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>4774.5</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="1"/>
+        <v>4774.5</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>9</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="2"/>
+      <c r="I11" s="1">
+        <f t="shared" si="4"/>
         <v>-13</v>
       </c>
+      <c r="J11" s="1">
+        <v>50</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>21</v>
       </c>
       <c r="B12" s="1">
-        <f>A12-11</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C12" s="1">
+        <f t="shared" si="2"/>
+        <v>71.018076644975068</v>
+      </c>
+      <c r="D12" s="1">
         <v>4801.7</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>4881.8</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>4841.75</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="1"/>
+        <v>4841.75</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="3"/>
         <v>80.100000000000364</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>10</v>
       </c>
-      <c r="H12">
-        <f t="shared" si="2"/>
+      <c r="I12" s="1">
+        <f t="shared" si="4"/>
         <v>-12.300000000000182</v>
       </c>
+      <c r="J12" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>22</v>
       </c>
       <c r="B13" s="1">
-        <f>A13-11</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C13" s="1">
+        <f t="shared" si="2"/>
+        <v>69.973314606740857</v>
+      </c>
+      <c r="D13" s="1">
         <v>4870.3</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>4951.5</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>4910.8999999999996</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="1"/>
+        <v>4910.8999999999996</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="3"/>
         <v>81.199999999999818</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>10</v>
       </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
+      <c r="I13" s="1">
+        <f t="shared" si="4"/>
         <v>-11.5</v>
       </c>
+      <c r="J13" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>23</v>
       </c>
       <c r="B14" s="1">
-        <f>A14-11</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C14" s="1">
+        <f t="shared" si="2"/>
+        <v>68.968622100955656</v>
+      </c>
+      <c r="D14" s="1">
         <v>4940.8999999999996</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>5023.3</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="0"/>
-        <v>4982.1000000000004</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="1"/>
+        <v>4982.1000000000004</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="3"/>
         <v>82.400000000000546</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>13</v>
       </c>
-      <c r="H14">
-        <f t="shared" si="2"/>
+      <c r="I14" s="1">
+        <f t="shared" si="4"/>
         <v>-10.600000000000364</v>
       </c>
+      <c r="J14" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>24</v>
       </c>
       <c r="B15" s="1">
-        <f>A15-11</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C15" s="1">
+        <f t="shared" si="2"/>
+        <v>68.003313452616979</v>
+      </c>
+      <c r="D15" s="1">
         <v>5013.5</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>5097.3</v>
-      </c>
-      <c r="E15" s="1">
-        <f t="shared" si="0"/>
-        <v>5055.3999999999996</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
+        <v>5055.3999999999996</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="3"/>
         <v>83.800000000000182</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>12</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
+      <c r="I15" s="1">
+        <f t="shared" si="4"/>
         <v>-9.8000000000001819</v>
       </c>
+      <c r="J15" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>25</v>
       </c>
       <c r="B16" s="1">
-        <f>A16-11</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C16" s="1">
+        <f t="shared" si="2"/>
+        <v>66.949228791774402</v>
+      </c>
+      <c r="D16" s="1">
         <v>5088.3999999999996</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>5173.3</v>
-      </c>
-      <c r="E16" s="1">
-        <f t="shared" si="0"/>
-        <v>5130.8500000000004</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="1"/>
+        <v>5130.8500000000004</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="3"/>
         <v>84.900000000000546</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>11</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="2"/>
+      <c r="I16" s="1">
+        <f t="shared" si="4"/>
         <v>-8.9000000000005457</v>
       </c>
+      <c r="J16" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>26</v>
       </c>
       <c r="B17" s="1">
-        <f>A17-11</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C17" s="1">
+        <f t="shared" si="2"/>
+        <v>66.067457838850572</v>
+      </c>
+      <c r="D17" s="1">
         <v>5165.6000000000004</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>5251.7</v>
-      </c>
-      <c r="E17" s="1">
-        <f t="shared" si="0"/>
-        <v>5208.6499999999996</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="1"/>
+        <v>5208.6499999999996</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="3"/>
         <v>86.099999999999454</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>7</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="2"/>
+      <c r="I17" s="1">
+        <f t="shared" si="4"/>
         <v>-7.6999999999998181</v>
       </c>
+      <c r="J17" s="1">
+        <v>50</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>27</v>
       </c>
       <c r="B18" s="1">
-        <f>A18-11</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C18" s="1">
+        <f t="shared" si="2"/>
+        <v>64.989110707803562</v>
+      </c>
+      <c r="D18" s="1">
         <v>5245</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>5332.4</v>
-      </c>
-      <c r="E18" s="1">
-        <f t="shared" si="0"/>
-        <v>5288.7</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="1"/>
+        <v>5288.7</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="3"/>
         <v>87.399999999999636</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>8</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="2"/>
+      <c r="I18" s="1">
+        <f t="shared" si="4"/>
         <v>-6.6999999999998181</v>
       </c>
+      <c r="J18" s="1">
+        <v>50</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>28</v>
       </c>
       <c r="B19" s="1">
-        <f>A19-11</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C19" s="1">
+        <f t="shared" si="2"/>
+        <v>64.118096357227202</v>
+      </c>
+      <c r="D19" s="1">
         <v>5326.9</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>5415.8</v>
-      </c>
-      <c r="E19" s="1">
-        <f t="shared" si="0"/>
-        <v>5371.35</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="1"/>
+        <v>5371.35</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="3"/>
         <v>88.900000000000546</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>8</v>
       </c>
-      <c r="H19">
+      <c r="I19" s="1">
+        <f t="shared" si="4"/>
+        <v>-5.5</v>
+      </c>
+      <c r="J19" s="1">
+        <v>50</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C20" s="1">
         <f t="shared" si="2"/>
-        <v>-5.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>29</v>
-      </c>
-      <c r="B20" s="1">
-        <f>A20-11</f>
-        <v>18</v>
-      </c>
-      <c r="C20" s="1">
+        <v>62.864512471655452</v>
+      </c>
+      <c r="D20" s="1">
         <v>5411.2</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>5501.7</v>
-      </c>
-      <c r="E20" s="1">
-        <f t="shared" si="0"/>
-        <v>5456.45</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="1"/>
+        <v>5456.45</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="3"/>
         <v>90.5</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>8</v>
       </c>
-      <c r="H20">
-        <f t="shared" si="2"/>
+      <c r="I20" s="1">
+        <f t="shared" si="4"/>
         <v>-4.6000000000003638</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>9</v>
+      <c r="J20" s="1">
+        <v>50</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>30</v>
       </c>
       <c r="B21" s="1">
-        <f>A21-11</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C21" s="1">
+        <f t="shared" si="2"/>
+        <v>62.030820033021214</v>
+      </c>
+      <c r="D21" s="1">
         <v>5498.8</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>5590.5</v>
-      </c>
-      <c r="E21" s="1">
-        <f t="shared" si="0"/>
-        <v>5544.65</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="1"/>
+        <v>5544.65</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="3"/>
         <v>91.699999999999818</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>10</v>
       </c>
-      <c r="H21">
-        <f t="shared" si="2"/>
+      <c r="I21" s="1">
+        <f t="shared" si="4"/>
         <v>-2.8999999999996362</v>
       </c>
+      <c r="J21" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>31</v>
       </c>
       <c r="B22" s="1">
-        <f>A22-11</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C22" s="1">
+        <f t="shared" si="2"/>
+        <v>60.984034060670105</v>
+      </c>
+      <c r="D22" s="1">
         <v>5588.9</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>5682.1</v>
-      </c>
-      <c r="E22" s="1">
-        <f t="shared" si="0"/>
-        <v>5635.5</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="1"/>
+        <v>5635.5</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="3"/>
         <v>93.200000000000728</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>10</v>
       </c>
-      <c r="H22">
-        <f t="shared" si="2"/>
+      <c r="I22" s="1">
+        <f t="shared" si="4"/>
         <v>-1.6000000000003638</v>
       </c>
+      <c r="J22" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>32</v>
       </c>
       <c r="B23" s="1">
-        <f>A23-11</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C23" s="1">
+        <f t="shared" si="2"/>
+        <v>59.97529593412272</v>
+      </c>
+      <c r="D23" s="1">
         <v>5682.1</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>5776.8</v>
-      </c>
-      <c r="E23" s="1">
-        <f t="shared" si="0"/>
-        <v>5729.4500000000007</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="1"/>
+        <v>5729.4500000000007</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="3"/>
         <v>94.699999999999818</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>13</v>
       </c>
-      <c r="H23">
+      <c r="I23" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>33</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="2"/>
+        <v>59.033864541832884</v>
+      </c>
+      <c r="D24" s="1">
+        <v>5778.4</v>
+      </c>
+      <c r="E24" s="1">
+        <v>5874.8</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>5826.6</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="3"/>
+        <v>96.400000000000546</v>
+      </c>
+      <c r="H24" s="1">
+        <v>10</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="4"/>
+        <v>1.5999999999994543</v>
+      </c>
+      <c r="J24" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>34</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="2"/>
+        <v>57.990384615384613</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5878</v>
+      </c>
+      <c r="E25" s="1">
+        <v>5976</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>5927</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+      <c r="H25" s="1">
+        <v>13</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="4"/>
+        <v>3.1999999999998181</v>
+      </c>
+      <c r="J25" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>35</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="2"/>
+        <v>57.024152345564517</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5981.1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>6080.9</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>6031</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="3"/>
+        <v>99.799999999999272</v>
+      </c>
+      <c r="H26" s="1">
+        <v>17</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="4"/>
+        <v>5.1000000000003638</v>
+      </c>
+      <c r="J26" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>36</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="2"/>
+        <v>55.98119122257026</v>
+      </c>
+      <c r="D27" s="1">
+        <v>6087.9</v>
+      </c>
+      <c r="E27" s="1">
+        <v>6189.4</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>6138.65</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="3"/>
+        <v>101.5</v>
+      </c>
+      <c r="H27" s="1">
+        <v>9</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="J27" s="1">
+        <v>50</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>37</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="2"/>
+        <v>54.998272138229368</v>
+      </c>
+      <c r="D28" s="1">
+        <v>6198.6</v>
+      </c>
+      <c r="E28" s="1">
+        <v>6302</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="1"/>
+        <v>6250.3</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="3"/>
+        <v>103.39999999999964</v>
+      </c>
+      <c r="H28" s="1">
+        <v>11</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="4"/>
+        <v>9.2000000000007276</v>
+      </c>
+      <c r="J28" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="2"/>
+        <v>54.006244796003166</v>
+      </c>
+      <c r="D29" s="1">
+        <v>6313.4</v>
+      </c>
+      <c r="E29" s="1">
+        <v>6418.7</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="1"/>
+        <v>6366.0499999999993</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="3"/>
+        <v>105.30000000000018</v>
+      </c>
+      <c r="H29" s="1">
+        <v>11</v>
+      </c>
+      <c r="I29" s="1">
+        <f>D29-E28</f>
+        <v>11.399999999999636</v>
+      </c>
+      <c r="J29" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>39</v>
+      </c>
+      <c r="B30" s="3">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="2"/>
+        <v>52.764964086192684</v>
+      </c>
+      <c r="D30" s="3">
+        <v>6432.5</v>
+      </c>
+      <c r="E30" s="3">
+        <v>6539.8</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="1"/>
+        <v>6486.15</v>
+      </c>
+      <c r="G30" s="3">
+        <f t="shared" si="3"/>
+        <v>107.30000000000018</v>
+      </c>
+      <c r="H30" s="3">
+        <v>13</v>
+      </c>
+      <c r="I30" s="3">
+        <f t="shared" si="4"/>
+        <v>13.800000000000182</v>
+      </c>
+      <c r="J30" s="4">
+        <v>20</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>40</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="2"/>
+        <v>52.271423032183456</v>
+      </c>
+      <c r="D31" s="1">
+        <v>6557.3</v>
+      </c>
+      <c r="E31" s="1">
+        <v>6665.6</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>6611.4500000000007</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="3"/>
+        <v>108.30000000000018</v>
+      </c>
+      <c r="H31" s="1">
+        <v>11</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="4"/>
+        <v>17.5</v>
+      </c>
+      <c r="J31" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>41</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" si="2"/>
+        <v>51.376681614349366</v>
+      </c>
+      <c r="D32" s="1">
+        <v>6684.6</v>
+      </c>
+      <c r="E32" s="1">
+        <v>6796.2</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="1"/>
+        <v>6740.4</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="3"/>
+        <v>111.59999999999945</v>
+      </c>
+      <c r="H32" s="1">
+        <v>14</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="J32" s="4">
+        <v>5</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>42</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" si="2"/>
+        <v>49.615275813295746</v>
+      </c>
+      <c r="D33" s="1">
+        <v>6818.1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>6930.3</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="1"/>
+        <v>6874.2000000000007</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="3"/>
+        <v>112.19999999999982</v>
+      </c>
+      <c r="H33" s="1">
+        <v>12</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="4"/>
+        <v>21.900000000000546</v>
+      </c>
+      <c r="J33" s="4">
+        <v>20</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>43</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C34" s="1">
+        <f t="shared" si="2"/>
+        <v>49.002736914129443</v>
+      </c>
+      <c r="D34" s="1">
+        <v>6957.6</v>
+      </c>
+      <c r="E34" s="1">
+        <v>7073.6</v>
+      </c>
+      <c r="F34" s="1">
+        <f>(E34+D34)/2</f>
+        <v>7015.6</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="3"/>
+        <v>116</v>
+      </c>
+      <c r="H34" s="1">
+        <v>10</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="4"/>
+        <v>27.300000000000182</v>
+      </c>
+      <c r="J34" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>44</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" si="2"/>
+        <v>47.993110236220588</v>
+      </c>
+      <c r="D35" s="1">
+        <v>7102.6</v>
+      </c>
+      <c r="E35" s="1">
+        <v>7220.9</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" ref="F35:F49" si="5">(E35+D35)/2</f>
+        <v>7161.75</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="3"/>
+        <v>118.29999999999927</v>
+      </c>
+      <c r="H35" s="1">
+        <v>10</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="J35" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>45</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" si="2"/>
+        <v>47.000943396226411</v>
+      </c>
+      <c r="D36" s="1">
+        <v>7253.7</v>
+      </c>
+      <c r="E36" s="1">
+        <v>7374.6</v>
+      </c>
+      <c r="F36" s="1">
+        <f t="shared" si="5"/>
+        <v>7314.15</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="3"/>
+        <v>120.90000000000055</v>
+      </c>
+      <c r="H36" s="1">
+        <v>9</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="4"/>
+        <v>32.800000000000182</v>
+      </c>
+      <c r="J36" s="1">
+        <v>50</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>46</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" si="2"/>
+        <v>46.032539921662952</v>
+      </c>
+      <c r="D37" s="1">
+        <v>7411.4</v>
+      </c>
+      <c r="E37" s="1">
+        <v>7534.9</v>
+      </c>
+      <c r="F37" s="1">
+        <f t="shared" si="5"/>
+        <v>7473.15</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="3"/>
+        <v>123.5</v>
+      </c>
+      <c r="H37" s="1">
+        <v>14</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="4"/>
+        <v>36.799999999999272</v>
+      </c>
+      <c r="J37" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>47</v>
+      </c>
+      <c r="B38" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="2"/>
+        <v>44.714449213161664</v>
+      </c>
+      <c r="D38" s="1">
+        <v>7576</v>
+      </c>
+      <c r="E38" s="1">
+        <v>7702.2</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="5"/>
+        <v>7639.1</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="3"/>
+        <v>126.19999999999982</v>
+      </c>
+      <c r="H38" s="1">
+        <v>12</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="4"/>
+        <v>41.100000000000364</v>
+      </c>
+      <c r="J38" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>48</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="2"/>
+        <v>44.266057585825159</v>
+      </c>
+      <c r="D39" s="1">
+        <v>7750.3</v>
+      </c>
+      <c r="E39" s="1">
+        <v>7877.4</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="5"/>
+        <v>7813.85</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="3"/>
+        <v>127.09999999999945</v>
+      </c>
+      <c r="H39" s="1">
+        <v>9</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" si="4"/>
+        <v>48.100000000000364</v>
+      </c>
+      <c r="J39" s="1">
+        <v>50</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>49</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="2"/>
+        <v>42.855759162303464</v>
+      </c>
+      <c r="D40" s="1">
+        <v>7928.4</v>
+      </c>
+      <c r="E40" s="1">
+        <v>8060.5</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" si="5"/>
+        <v>7994.45</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="3"/>
+        <v>132.10000000000036</v>
+      </c>
+      <c r="H40" s="1">
+        <v>9</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="4"/>
+        <v>51</v>
+      </c>
+      <c r="J40" s="1">
+        <v>50</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
+        <v>50</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="2"/>
+        <v>42.143252073385128</v>
+      </c>
+      <c r="D41" s="1">
+        <v>8117.2</v>
+      </c>
+      <c r="E41" s="1">
+        <v>8253.7000000000007</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="5"/>
+        <v>8185.4500000000007</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="3"/>
+        <v>136.50000000000091</v>
+      </c>
+      <c r="H41" s="1">
+        <v>8</v>
+      </c>
+      <c r="I41" s="1">
+        <f t="shared" si="4"/>
+        <v>56.699999999999818</v>
+      </c>
+      <c r="J41" s="4">
+        <v>5</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>51</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="2"/>
+        <v>41.021002386635196</v>
+      </c>
+      <c r="D42" s="1">
+        <v>8315.1</v>
+      </c>
+      <c r="E42" s="1">
+        <v>8453.7000000000007</v>
+      </c>
+      <c r="F42" s="1">
+        <f t="shared" si="5"/>
+        <v>8384.4000000000015</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="3"/>
+        <v>138.60000000000036</v>
+      </c>
+      <c r="H42" s="1">
+        <v>10</v>
+      </c>
+      <c r="I42" s="1">
+        <f t="shared" si="4"/>
+        <v>61.399999999999636</v>
+      </c>
+      <c r="J42" s="4">
+        <v>5</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>52</v>
+      </c>
+      <c r="B43" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="2"/>
+        <v>39.798645598193808</v>
+      </c>
+      <c r="D43" s="1">
+        <v>8522.9</v>
+      </c>
+      <c r="E43" s="1">
+        <v>8664.9</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="5"/>
+        <v>8593.9</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="3"/>
+        <v>142</v>
+      </c>
+      <c r="H43" s="1">
+        <v>6</v>
+      </c>
+      <c r="I43" s="1">
+        <f t="shared" si="4"/>
+        <v>69.199999999998909</v>
+      </c>
+      <c r="J43" s="1">
+        <v>50</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>53</v>
+      </c>
+      <c r="B44" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="2"/>
+        <v>39.170166702749697</v>
+      </c>
+      <c r="D44" s="1">
+        <v>8741.6</v>
+      </c>
+      <c r="E44" s="1">
+        <v>8889.2000000000007</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="5"/>
+        <v>8815.4000000000015</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="3"/>
+        <v>147.60000000000036</v>
+      </c>
+      <c r="H44" s="1">
+        <v>10</v>
+      </c>
+      <c r="I44" s="1">
+        <f t="shared" si="4"/>
+        <v>76.700000000000728</v>
+      </c>
+      <c r="J44" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>54</v>
+      </c>
+      <c r="B45" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="2"/>
+        <v>38.037256908905086</v>
+      </c>
+      <c r="D45" s="1">
+        <v>8971.7000000000007</v>
+      </c>
+      <c r="E45" s="1">
+        <v>9121</v>
+      </c>
+      <c r="F45" s="1">
+        <f t="shared" si="5"/>
+        <v>9046.35</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="3"/>
+        <v>149.29999999999927</v>
+      </c>
+      <c r="H45" s="1">
+        <v>14</v>
+      </c>
+      <c r="I45" s="1">
+        <f t="shared" si="4"/>
+        <v>82.5</v>
+      </c>
+      <c r="J45" s="4">
+        <v>5</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>55</v>
+      </c>
+      <c r="B46" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="2"/>
+        <v>37.031025790187783</v>
+      </c>
+      <c r="D46" s="1">
+        <v>9213.9</v>
+      </c>
+      <c r="E46" s="1">
+        <v>9367.2999999999993</v>
+      </c>
+      <c r="F46" s="1">
+        <f t="shared" si="5"/>
+        <v>9290.5999999999985</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="3"/>
+        <v>153.39999999999964</v>
+      </c>
+      <c r="H46" s="1">
+        <v>7</v>
+      </c>
+      <c r="I46" s="1">
+        <f t="shared" si="4"/>
+        <v>92.899999999999636</v>
+      </c>
+      <c r="J46" s="1">
+        <v>50</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>56</v>
+      </c>
+      <c r="B47" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C47" s="1">
+        <f t="shared" si="2"/>
+        <v>36.033755274261701</v>
+      </c>
+      <c r="D47" s="1">
+        <v>9469.9</v>
+      </c>
+      <c r="E47" s="1">
+        <v>9627</v>
+      </c>
+      <c r="F47" s="1">
+        <f t="shared" si="5"/>
+        <v>9548.4500000000007</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="3"/>
+        <v>157.10000000000036</v>
+      </c>
+      <c r="H47" s="1">
+        <v>6</v>
+      </c>
+      <c r="I47" s="1">
+        <f t="shared" si="4"/>
+        <v>102.60000000000036</v>
+      </c>
+      <c r="J47" s="4">
+        <v>20</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>57</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="C48" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="D48" s="1">
+        <v>9740.4</v>
+      </c>
+      <c r="E48" s="1">
+        <v>9901.6</v>
+      </c>
+      <c r="F48" s="1">
+        <f t="shared" si="5"/>
+        <v>9821</v>
+      </c>
+      <c r="G48" s="1">
+        <f t="shared" si="3"/>
+        <v>161.20000000000073</v>
+      </c>
+      <c r="H48" s="1">
+        <v>6</v>
+      </c>
+      <c r="I48" s="1">
+        <f t="shared" si="4"/>
+        <v>113.39999999999964</v>
+      </c>
+      <c r="J48" s="3">
+        <v>50</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>33</v>
-      </c>
-      <c r="B24" s="1">
-        <f>A24-11</f>
-        <v>22</v>
-      </c>
-      <c r="C24" s="1">
-        <v>5778.4</v>
-      </c>
-      <c r="D24" s="1">
-        <v>5874.8</v>
-      </c>
-      <c r="E24" s="1">
-        <f t="shared" si="0"/>
-        <v>5826.6</v>
-      </c>
-      <c r="F24" s="1">
-        <f t="shared" si="1"/>
-        <v>96.400000000000546</v>
-      </c>
-      <c r="G24" s="1">
-        <v>10</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="2"/>
-        <v>1.5999999999994543</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>34</v>
-      </c>
-      <c r="B25" s="1">
-        <f>A25-11</f>
-        <v>23</v>
-      </c>
-      <c r="C25" s="1">
-        <v>5878</v>
-      </c>
-      <c r="D25" s="1">
-        <v>5976</v>
-      </c>
-      <c r="E25" s="1">
-        <f t="shared" si="0"/>
-        <v>5927</v>
-      </c>
-      <c r="F25" s="1">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-      <c r="G25" s="1">
-        <v>13</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="2"/>
-        <v>3.1999999999998181</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>35</v>
-      </c>
-      <c r="B26" s="1">
-        <f>A26-11</f>
-        <v>24</v>
-      </c>
-      <c r="C26" s="1">
-        <v>5981.1</v>
-      </c>
-      <c r="D26" s="1">
-        <v>6080.9</v>
-      </c>
-      <c r="E26" s="1">
-        <f t="shared" si="0"/>
-        <v>6031</v>
-      </c>
-      <c r="F26" s="1">
-        <f t="shared" si="1"/>
-        <v>99.799999999999272</v>
-      </c>
-      <c r="G26" s="1">
-        <v>17</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="2"/>
-        <v>5.1000000000003638</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>36</v>
-      </c>
-      <c r="B27" s="1">
-        <f>A27-11</f>
-        <v>25</v>
-      </c>
-      <c r="C27" s="1">
-        <v>6087.9</v>
-      </c>
-      <c r="D27" s="1">
-        <v>6189.4</v>
-      </c>
-      <c r="E27" s="1">
-        <f t="shared" si="0"/>
-        <v>6138.65</v>
-      </c>
-      <c r="F27" s="1">
-        <f t="shared" si="1"/>
-        <v>101.5</v>
-      </c>
-      <c r="G27" s="1">
-        <v>9</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>37</v>
-      </c>
-      <c r="B28" s="1">
-        <f>A28-11</f>
-        <v>26</v>
-      </c>
-      <c r="C28" s="1">
-        <v>6198.6</v>
-      </c>
-      <c r="D28" s="1">
-        <v>6302</v>
-      </c>
-      <c r="E28" s="1">
-        <f t="shared" si="0"/>
-        <v>6250.3</v>
-      </c>
-      <c r="F28" s="1">
-        <f t="shared" si="1"/>
-        <v>103.39999999999964</v>
-      </c>
-      <c r="G28" s="1">
-        <v>11</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="2"/>
-        <v>9.2000000000007276</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>38</v>
-      </c>
-      <c r="B29" s="1">
-        <f>A29-11</f>
-        <v>27</v>
-      </c>
-      <c r="C29" s="1">
-        <v>6313.4</v>
-      </c>
-      <c r="D29" s="1">
-        <v>6418.7</v>
-      </c>
-      <c r="E29" s="1">
-        <f t="shared" si="0"/>
-        <v>6366.0499999999993</v>
-      </c>
-      <c r="F29" s="1">
-        <f t="shared" si="1"/>
-        <v>105.30000000000018</v>
-      </c>
-      <c r="G29" s="1">
-        <v>11</v>
-      </c>
-      <c r="H29">
-        <f>C29-D28</f>
-        <v>11.399999999999636</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>39</v>
-      </c>
-      <c r="B30" s="2">
-        <f>A30-11</f>
-        <v>28</v>
-      </c>
-      <c r="C30" s="2">
-        <v>6434.2</v>
-      </c>
-      <c r="D30" s="2">
-        <v>6540</v>
-      </c>
-      <c r="E30" s="2">
-        <f t="shared" si="0"/>
-        <v>6487.1</v>
-      </c>
-      <c r="F30" s="2">
-        <f t="shared" si="1"/>
-        <v>105.80000000000018</v>
-      </c>
-      <c r="G30" s="2">
-        <v>13</v>
-      </c>
-      <c r="H30" s="3">
-        <f t="shared" si="2"/>
-        <v>15.5</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>40</v>
-      </c>
-      <c r="B31" s="1">
-        <f>A31-11</f>
-        <v>29</v>
-      </c>
-      <c r="C31" s="1">
-        <v>6557.3</v>
-      </c>
-      <c r="D31" s="1">
-        <v>6665.6</v>
-      </c>
-      <c r="E31" s="1">
-        <f t="shared" si="0"/>
-        <v>6611.4500000000007</v>
-      </c>
-      <c r="F31" s="1">
-        <f t="shared" si="1"/>
-        <v>108.30000000000018</v>
-      </c>
-      <c r="G31" s="1">
-        <v>11</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="2"/>
-        <v>17.300000000000182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>41</v>
-      </c>
-      <c r="B32" s="1">
-        <f>A32-11</f>
-        <v>30</v>
-      </c>
-      <c r="C32" s="1">
-        <v>6681.3</v>
-      </c>
-      <c r="D32" s="1">
-        <v>6795.7</v>
-      </c>
-      <c r="E32" s="1">
-        <f t="shared" si="0"/>
-        <v>6738.5</v>
-      </c>
-      <c r="F32" s="1">
-        <f t="shared" si="1"/>
-        <v>114.39999999999964</v>
-      </c>
-      <c r="G32" s="1">
-        <v>8</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="2"/>
-        <v>15.699999999999818</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>42</v>
-      </c>
-      <c r="B33" s="1">
-        <f>A33-11</f>
-        <v>31</v>
-      </c>
-      <c r="C33" s="1">
-        <v>6816.9</v>
-      </c>
-      <c r="D33" s="1">
-        <v>6929.8</v>
-      </c>
-      <c r="E33" s="1">
-        <f t="shared" si="0"/>
-        <v>6873.35</v>
-      </c>
-      <c r="F33" s="1">
-        <f t="shared" si="1"/>
-        <v>112.90000000000055</v>
-      </c>
-      <c r="G33" s="1">
-        <v>7</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="2"/>
-        <v>21.199999999999818</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>43</v>
-      </c>
-      <c r="B34" s="1">
-        <f>A34-11</f>
-        <v>32</v>
-      </c>
-      <c r="C34" s="1">
-        <v>6957.6</v>
-      </c>
-      <c r="D34" s="1">
-        <v>7073.6</v>
-      </c>
-      <c r="E34" s="1">
-        <f>(D34+C34)/2</f>
-        <v>7015.6</v>
-      </c>
-      <c r="F34" s="1">
-        <f t="shared" si="1"/>
-        <v>116</v>
-      </c>
-      <c r="G34" s="1">
-        <v>10</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="2"/>
-        <v>27.800000000000182</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>44</v>
-      </c>
-      <c r="B35" s="1">
-        <f>A35-11</f>
-        <v>33</v>
-      </c>
-      <c r="C35" s="1">
-        <v>7102.6</v>
-      </c>
-      <c r="D35" s="1">
-        <v>7220.9</v>
-      </c>
-      <c r="E35" s="1">
-        <f t="shared" ref="E35:E49" si="3">(D35+C35)/2</f>
-        <v>7161.75</v>
-      </c>
-      <c r="F35" s="1">
-        <f t="shared" si="1"/>
-        <v>118.29999999999927</v>
-      </c>
-      <c r="G35" s="1">
-        <v>10</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>45</v>
-      </c>
-      <c r="B36" s="1">
-        <f>A36-11</f>
-        <v>34</v>
-      </c>
-      <c r="C36" s="1">
-        <v>7253.7</v>
-      </c>
-      <c r="D36" s="1">
-        <v>7374.6</v>
-      </c>
-      <c r="E36" s="1">
-        <f t="shared" si="3"/>
-        <v>7314.15</v>
-      </c>
-      <c r="F36" s="1">
-        <f t="shared" si="1"/>
-        <v>120.90000000000055</v>
-      </c>
-      <c r="G36" s="1">
-        <v>9</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="2"/>
-        <v>32.800000000000182</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>46</v>
-      </c>
-      <c r="B37" s="1">
-        <f>A37-11</f>
-        <v>35</v>
-      </c>
-      <c r="C37" s="1">
-        <v>7411.4</v>
-      </c>
-      <c r="D37" s="1">
-        <v>7534.9</v>
-      </c>
-      <c r="E37" s="1">
-        <f t="shared" si="3"/>
-        <v>7473.15</v>
-      </c>
-      <c r="F37" s="1">
-        <f t="shared" si="1"/>
-        <v>123.5</v>
-      </c>
-      <c r="G37" s="1">
-        <v>14</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="2"/>
-        <v>36.799999999999272</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>47</v>
-      </c>
-      <c r="B38" s="1">
-        <f>A38-11</f>
-        <v>36</v>
-      </c>
-      <c r="C38" s="1">
-        <v>7576</v>
-      </c>
-      <c r="D38" s="1">
-        <v>7702.2</v>
-      </c>
-      <c r="E38" s="1">
-        <f t="shared" si="3"/>
-        <v>7639.1</v>
-      </c>
-      <c r="F38" s="1">
-        <f t="shared" si="1"/>
-        <v>126.19999999999982</v>
-      </c>
-      <c r="G38" s="1">
-        <v>12</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="2"/>
-        <v>41.100000000000364</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>48</v>
-      </c>
-      <c r="B39" s="1">
-        <f>A39-11</f>
-        <v>37</v>
-      </c>
-      <c r="C39" s="1">
-        <v>7750.3</v>
-      </c>
-      <c r="D39" s="1">
-        <v>7877.4</v>
-      </c>
-      <c r="E39" s="1">
-        <f t="shared" si="3"/>
-        <v>7813.85</v>
-      </c>
-      <c r="F39" s="1">
-        <f t="shared" si="1"/>
-        <v>127.09999999999945</v>
-      </c>
-      <c r="G39" s="1">
-        <v>9</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="2"/>
-        <v>48.100000000000364</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>49</v>
-      </c>
-      <c r="B40" s="1">
-        <f>A40-11</f>
-        <v>38</v>
-      </c>
-      <c r="C40" s="1">
-        <v>7928.4</v>
-      </c>
-      <c r="D40" s="1">
-        <v>8060.5</v>
-      </c>
-      <c r="E40" s="1">
-        <f t="shared" si="3"/>
-        <v>7994.45</v>
-      </c>
-      <c r="F40" s="1">
-        <f t="shared" si="1"/>
-        <v>132.10000000000036</v>
-      </c>
-      <c r="G40" s="1">
-        <v>9</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="2"/>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>50</v>
-      </c>
-      <c r="B41" s="1">
-        <f>A41-11</f>
-        <v>39</v>
-      </c>
-      <c r="C41" s="1">
-        <v>8117</v>
-      </c>
-      <c r="D41" s="1">
-        <v>8230.6</v>
-      </c>
-      <c r="E41" s="1">
-        <f t="shared" si="3"/>
-        <v>8173.8</v>
-      </c>
-      <c r="F41" s="1">
-        <f t="shared" si="1"/>
-        <v>113.60000000000036</v>
-      </c>
-      <c r="G41" s="1">
-        <v>8</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="2"/>
-        <v>56.5</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>51</v>
-      </c>
-      <c r="B42" s="1">
-        <f>A42-11</f>
-        <v>40</v>
-      </c>
-      <c r="C42" s="1">
-        <v>8315.1</v>
-      </c>
-      <c r="D42" s="1">
-        <v>8454.9</v>
-      </c>
-      <c r="E42" s="1">
-        <f t="shared" si="3"/>
-        <v>8385</v>
-      </c>
-      <c r="F42" s="1">
-        <f t="shared" si="1"/>
-        <v>139.79999999999927</v>
-      </c>
-      <c r="G42" s="1">
-        <v>10</v>
-      </c>
-      <c r="H42">
-        <f t="shared" si="2"/>
-        <v>84.5</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <v>52</v>
-      </c>
-      <c r="B43" s="1">
-        <f>A43-11</f>
-        <v>41</v>
-      </c>
-      <c r="C43" s="1">
-        <v>8522.9</v>
-      </c>
-      <c r="D43" s="1">
-        <v>8664.9</v>
-      </c>
-      <c r="E43" s="1">
-        <f t="shared" si="3"/>
-        <v>8593.9</v>
-      </c>
-      <c r="F43" s="1">
-        <f t="shared" si="1"/>
-        <v>142</v>
-      </c>
-      <c r="G43" s="1">
-        <v>6</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
-        <v>53</v>
-      </c>
-      <c r="B44" s="1">
-        <f>A44-11</f>
-        <v>42</v>
-      </c>
-      <c r="C44" s="1">
-        <v>8741.6</v>
-      </c>
-      <c r="D44" s="1">
-        <v>8889.2000000000007</v>
-      </c>
-      <c r="E44" s="1">
-        <f t="shared" si="3"/>
-        <v>8815.4000000000015</v>
-      </c>
-      <c r="F44" s="1">
-        <f t="shared" si="1"/>
-        <v>147.60000000000036</v>
-      </c>
-      <c r="G44" s="1">
-        <v>10</v>
-      </c>
-      <c r="H44">
-        <f t="shared" si="2"/>
-        <v>76.700000000000728</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
-        <v>54</v>
-      </c>
-      <c r="B45" s="1">
-        <f>A45-11</f>
-        <v>43</v>
-      </c>
-      <c r="C45" s="1">
-        <v>8968</v>
-      </c>
-      <c r="D45" s="1">
-        <v>9116.7999999999993</v>
-      </c>
-      <c r="E45" s="1">
-        <f t="shared" si="3"/>
-        <v>9042.4</v>
-      </c>
-      <c r="F45" s="1">
-        <f t="shared" si="1"/>
-        <v>148.79999999999927</v>
-      </c>
-      <c r="G45" s="1">
-        <v>9</v>
-      </c>
-      <c r="H45">
-        <f t="shared" si="2"/>
-        <v>78.799999999999272</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
-        <v>55</v>
-      </c>
-      <c r="B46" s="1">
-        <f>A46-11</f>
-        <v>44</v>
-      </c>
-      <c r="C46" s="1">
-        <v>9213.9</v>
-      </c>
-      <c r="D46" s="1">
-        <v>9367.2999999999993</v>
-      </c>
-      <c r="E46" s="1">
-        <f t="shared" si="3"/>
-        <v>9290.5999999999985</v>
-      </c>
-      <c r="F46" s="1">
-        <f t="shared" si="1"/>
-        <v>153.39999999999964</v>
-      </c>
-      <c r="G46" s="1">
-        <v>7</v>
-      </c>
-      <c r="H46">
-        <f t="shared" si="2"/>
-        <v>97.100000000000364</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
-        <v>56</v>
-      </c>
-      <c r="B47" s="1">
-        <f>A47-11</f>
-        <v>45</v>
-      </c>
-      <c r="C47" s="1">
-        <v>9469.9</v>
-      </c>
-      <c r="D47" s="1">
-        <v>9624.6</v>
-      </c>
-      <c r="E47" s="1">
-        <f t="shared" si="3"/>
-        <v>9547.25</v>
-      </c>
-      <c r="F47" s="1">
-        <f t="shared" si="1"/>
-        <v>154.70000000000073</v>
-      </c>
-      <c r="G47" s="1">
-        <v>6</v>
-      </c>
-      <c r="H47">
-        <f t="shared" si="2"/>
-        <v>102.60000000000036</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <v>57</v>
-      </c>
-      <c r="B48" s="1">
-        <f>A48-11</f>
-        <v>46</v>
-      </c>
-      <c r="C48" s="1">
-        <v>9740.4</v>
-      </c>
-      <c r="D48" s="1">
-        <v>9901.6</v>
-      </c>
-      <c r="E48" s="1">
-        <f t="shared" si="3"/>
-        <v>9821</v>
-      </c>
-      <c r="F48" s="1">
-        <f t="shared" si="1"/>
-        <v>161.20000000000073</v>
-      </c>
-      <c r="G48" s="1">
-        <v>6</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="2"/>
-        <v>115.79999999999927</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>58</v>
       </c>
       <c r="B49" s="1">
-        <f>A49-11</f>
+        <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="E49" s="1">
+      <c r="C49" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F49" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G49" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F49" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <f t="shared" si="2"/>
+      <c r="I49" s="1">
+        <f t="shared" si="4"/>
         <v>-9901.6</v>
       </c>
-      <c r="I49" s="1" t="s">
-        <v>16</v>
+      <c r="J49" s="1">
+        <v>50</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C51" s="1">
+        <f t="shared" ref="C51:C59" si="6">F52/(F52-F51)</f>
+        <v>91.920903954803137</v>
+      </c>
+      <c r="D51" s="1">
+        <f>F51-G51/2</f>
+        <v>3704.9660138291279</v>
+      </c>
+      <c r="E51" s="1">
+        <f>F51+G51/2</f>
+        <v>3766.9390138291278</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" ref="F51:F59" si="7">C52*F52/(C52+1)</f>
+        <v>3735.9525138291278</v>
+      </c>
+      <c r="G51" s="1">
+        <f>0.000007*A51^4-0.0004*A51^3+0.0185*A51^2+0.5793*A51+61.973</f>
+        <v>61.972999999999999</v>
+      </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>1</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C52" s="1">
+        <f t="shared" si="6"/>
+        <v>90.920903954802228</v>
+      </c>
+      <c r="D52" s="1">
+        <f t="shared" ref="D52:D61" si="8">F52-G52/2</f>
+        <v>3745.7574485847513</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" ref="E52:E61" si="9">F52+G52/2</f>
+        <v>3808.3278555847514</v>
+      </c>
+      <c r="F52" s="1">
+        <f t="shared" si="7"/>
+        <v>3777.0426520847514</v>
+      </c>
+      <c r="G52" s="1">
+        <f t="shared" ref="G52:G61" si="10">0.000007*A52^4-0.0004*A52^3+0.0185*A52^2+0.5793*A52+61.973</f>
+        <v>62.570406999999996</v>
+      </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>2</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C53" s="1">
+        <f t="shared" si="6"/>
+        <v>89.92090395480156</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" si="8"/>
+        <v>3787.4454517155004</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="9"/>
+        <v>3850.6479637155003</v>
+      </c>
+      <c r="F53" s="1">
+        <f t="shared" si="7"/>
+        <v>3819.0467077155004</v>
+      </c>
+      <c r="G53" s="1">
+        <f t="shared" si="10"/>
+        <v>63.202511999999999</v>
+      </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>3</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C54" s="1">
+        <f t="shared" si="6"/>
+        <v>88.920903954801304</v>
+      </c>
+      <c r="D54" s="1">
+        <f t="shared" si="8"/>
+        <v>3830.0619308274609</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="9"/>
+        <v>3893.9290978274612</v>
+      </c>
+      <c r="F54" s="1">
+        <f t="shared" si="7"/>
+        <v>3861.995514327461</v>
+      </c>
+      <c r="G54" s="1">
+        <f t="shared" si="10"/>
+        <v>63.867167000000002</v>
+      </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>4</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C55" s="1">
+        <f t="shared" si="6"/>
+        <v>87.920903954800934</v>
+      </c>
+      <c r="D55" s="1">
+        <f t="shared" si="8"/>
+        <v>3873.6401123151213</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="9"/>
+        <v>3938.2025043151211</v>
+      </c>
+      <c r="F55" s="1">
+        <f t="shared" si="7"/>
+        <v>3905.9213083151212</v>
+      </c>
+      <c r="G55" s="1">
+        <f t="shared" si="10"/>
+        <v>64.562392000000003</v>
+      </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>5</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C56" s="1">
+        <f t="shared" si="6"/>
+        <v>86.92090395480119</v>
+      </c>
+      <c r="D56" s="1">
+        <f t="shared" si="8"/>
+        <v>3918.2146220547565</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="9"/>
+        <v>3983.5009970547562</v>
+      </c>
+      <c r="F56" s="1">
+        <f t="shared" si="7"/>
+        <v>3950.8578095547564</v>
+      </c>
+      <c r="G56" s="1">
+        <f t="shared" si="10"/>
+        <v>65.286374999999992</v>
+      </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C57" s="1">
+        <f t="shared" si="6"/>
+        <v>85.920903954801702</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="8"/>
+        <v>3963.821571732768</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="9"/>
+        <v>4029.859043732768</v>
+      </c>
+      <c r="F57" s="1">
+        <f t="shared" si="7"/>
+        <v>3996.840307732768</v>
+      </c>
+      <c r="G57" s="1">
+        <f t="shared" si="10"/>
+        <v>66.037471999999994</v>
+      </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>7</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C58" s="1">
+        <f t="shared" si="6"/>
+        <v>84.920903954801361</v>
+      </c>
+      <c r="D58" s="1">
+        <f t="shared" si="8"/>
+        <v>4010.498651273464</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="9"/>
+        <v>4077.3128582734644</v>
+      </c>
+      <c r="F58" s="1">
+        <f t="shared" si="7"/>
+        <v>4043.9057547734642</v>
+      </c>
+      <c r="G58" s="1">
+        <f t="shared" si="10"/>
+        <v>66.814206999999996</v>
+      </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>8</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C59" s="1">
+        <f t="shared" si="6"/>
+        <v>83.920903954800693</v>
+      </c>
+      <c r="D59" s="1">
+        <f t="shared" si="8"/>
+        <v>4058.285227875047</v>
+      </c>
+      <c r="E59" s="1">
+        <f t="shared" si="9"/>
+        <v>4125.900499875047</v>
+      </c>
+      <c r="F59" s="1">
+        <f t="shared" si="7"/>
+        <v>4092.092863875047</v>
+      </c>
+      <c r="G59" s="1">
+        <f t="shared" si="10"/>
+        <v>67.615272000000004</v>
+      </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>9</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C60" s="1">
+        <f>F61/(F61-F60)</f>
+        <v>82.920903954800565</v>
+      </c>
+      <c r="D60" s="1">
+        <f t="shared" si="8"/>
+        <v>4107.2224522116549</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" si="9"/>
+        <v>4175.6619792116553</v>
+      </c>
+      <c r="F60" s="1">
+        <f>C61*F61/(C61+1)</f>
+        <v>4141.4422157116551</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" si="10"/>
+        <v>68.439526999999998</v>
+      </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>10</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C61" s="1">
+        <f>F2/(F2-F61)</f>
+        <v>81.920903954800863</v>
+      </c>
+      <c r="D61" s="1">
+        <f t="shared" si="8"/>
+        <v>4157.3533724137915</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="9"/>
+        <v>4226.6393724137915</v>
+      </c>
+      <c r="F61" s="1">
+        <f>C2*F2/(C2+1)</f>
+        <v>4191.9963724137915</v>
+      </c>
+      <c r="G61" s="1">
+        <f t="shared" si="10"/>
+        <v>69.286000000000001</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:H1">
+  <conditionalFormatting sqref="H1:J1">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -5580,7 +6315,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G49">
+  <conditionalFormatting sqref="H2:H49">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>10</formula>
     </cfRule>

</xml_diff>

<commit_message>
Changed click events to key press events. Changed wave range in excel sheet for extrapolated orders.
</commit_message>
<xml_diff>
--- a/OrderInfo.xlsx
+++ b/OrderInfo.xlsx
@@ -630,11 +630,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-975726480"/>
-        <c:axId val="-975721680"/>
+        <c:axId val="-1734842560"/>
+        <c:axId val="-1734837760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-975726480"/>
+        <c:axId val="-1734842560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -691,12 +691,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-975721680"/>
+        <c:crossAx val="-1734837760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-975721680"/>
+        <c:axId val="-1734837760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -754,7 +754,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-975726480"/>
+        <c:crossAx val="-1734842560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1315,11 +1315,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-975691744"/>
-        <c:axId val="-975686944"/>
+        <c:axId val="-1734756752"/>
+        <c:axId val="-1734751952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-975691744"/>
+        <c:axId val="-1734756752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1375,12 +1375,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-975686944"/>
+        <c:crossAx val="-1734751952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-975686944"/>
+        <c:axId val="-1734751952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60.0"/>
@@ -1437,7 +1437,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-975691744"/>
+        <c:crossAx val="-1734756752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1910,11 +1910,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-975626272"/>
-        <c:axId val="-975621472"/>
+        <c:axId val="-1734714528"/>
+        <c:axId val="-1734709728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-975626272"/>
+        <c:axId val="-1734714528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1970,12 +1970,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-975621472"/>
+        <c:crossAx val="-1734709728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-975621472"/>
+        <c:axId val="-1734709728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -2034,7 +2034,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-975626272"/>
+        <c:crossAx val="-1734714528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4111,8 +4111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6021,6 +6021,18 @@
         <f>0.000007*A51^4-0.0004*A51^3+0.0185*A51^2+0.5793*A51+61.973</f>
         <v>61.972999999999999</v>
       </c>
+      <c r="H51" s="1">
+        <f>F51/60000/2</f>
+        <v>3.1132937615242731E-2</v>
+      </c>
+      <c r="I51" s="1">
+        <f>F51-H51*1024</f>
+        <v>3704.0723857111193</v>
+      </c>
+      <c r="J51" s="1">
+        <f>F51+H51*1024</f>
+        <v>3767.8326419471364</v>
+      </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
@@ -6049,6 +6061,18 @@
         <f t="shared" ref="G52:G61" si="10">0.000007*A52^4-0.0004*A52^3+0.0185*A52^2+0.5793*A52+61.973</f>
         <v>62.570406999999996</v>
       </c>
+      <c r="H52" s="1">
+        <f>F52/60000/2</f>
+        <v>3.1475355434039592E-2</v>
+      </c>
+      <c r="I52" s="1">
+        <f>F52-H52*1024</f>
+        <v>3744.811888120295</v>
+      </c>
+      <c r="J52" s="1">
+        <f t="shared" ref="J52:J61" si="11">F52+H52*1024</f>
+        <v>3809.2734160492078</v>
+      </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
@@ -6077,6 +6101,18 @@
         <f t="shared" si="10"/>
         <v>63.202511999999999</v>
       </c>
+      <c r="H53" s="1">
+        <f>F53/60000/2</f>
+        <v>3.1825389230962502E-2</v>
+      </c>
+      <c r="I53" s="1">
+        <f>F53-H53*1024</f>
+        <v>3786.4575091429947</v>
+      </c>
+      <c r="J53" s="1">
+        <f t="shared" si="11"/>
+        <v>3851.635906288006</v>
+      </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
@@ -6105,6 +6141,18 @@
         <f t="shared" si="10"/>
         <v>63.867167000000002</v>
       </c>
+      <c r="H54" s="1">
+        <f>F54/60000/2</f>
+        <v>3.2183295952728841E-2</v>
+      </c>
+      <c r="I54" s="1">
+        <f>F54-H54*1024</f>
+        <v>3829.0398192718667</v>
+      </c>
+      <c r="J54" s="1">
+        <f t="shared" si="11"/>
+        <v>3894.9512093830554</v>
+      </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
@@ -6133,6 +6181,18 @@
         <f t="shared" si="10"/>
         <v>64.562392000000003</v>
       </c>
+      <c r="H55" s="1">
+        <f>F55/60000/2</f>
+        <v>3.2549344235959343E-2</v>
+      </c>
+      <c r="I55" s="1">
+        <f>F55-H55*1024</f>
+        <v>3872.590779817499</v>
+      </c>
+      <c r="J55" s="1">
+        <f t="shared" si="11"/>
+        <v>3939.2518368127435</v>
+      </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
@@ -6161,6 +6221,18 @@
         <f t="shared" si="10"/>
         <v>65.286374999999992</v>
       </c>
+      <c r="H56" s="1">
+        <f>F56/60000/2</f>
+        <v>3.292381507962297E-2</v>
+      </c>
+      <c r="I56" s="1">
+        <f>F56-H56*1024</f>
+        <v>3917.1438229132223</v>
+      </c>
+      <c r="J56" s="1">
+        <f t="shared" si="11"/>
+        <v>3984.5717961962905</v>
+      </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
@@ -6189,6 +6261,18 @@
         <f t="shared" si="10"/>
         <v>66.037471999999994</v>
       </c>
+      <c r="H57" s="1">
+        <f>F57/60000/2</f>
+        <v>3.3307002564439733E-2</v>
+      </c>
+      <c r="I57" s="1">
+        <f>F57-H57*1024</f>
+        <v>3962.7339371067819</v>
+      </c>
+      <c r="J57" s="1">
+        <f t="shared" si="11"/>
+        <v>4030.9466783587541</v>
+      </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
@@ -6217,6 +6301,18 @@
         <f t="shared" si="10"/>
         <v>66.814206999999996</v>
       </c>
+      <c r="H58" s="1">
+        <f>F58/60000/2</f>
+        <v>3.3699214623112199E-2</v>
+      </c>
+      <c r="I58" s="1">
+        <f>F58-H58*1024</f>
+        <v>4009.3977589993974</v>
+      </c>
+      <c r="J58" s="1">
+        <f t="shared" si="11"/>
+        <v>4078.413750547531</v>
+      </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
@@ -6245,6 +6341,18 @@
         <f t="shared" si="10"/>
         <v>67.615272000000004</v>
       </c>
+      <c r="H59" s="1">
+        <f>F59/60000/2</f>
+        <v>3.4100773865625392E-2</v>
+      </c>
+      <c r="I59" s="1">
+        <f>F59-H59*1024</f>
+        <v>4057.1736714366466</v>
+      </c>
+      <c r="J59" s="1">
+        <f t="shared" si="11"/>
+        <v>4127.0120563134478</v>
+      </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
@@ -6273,6 +6381,18 @@
         <f t="shared" si="10"/>
         <v>68.439526999999998</v>
       </c>
+      <c r="H60" s="1">
+        <f>F60/60000/2</f>
+        <v>3.4512018464263793E-2</v>
+      </c>
+      <c r="I60" s="1">
+        <f>F60-H60*1024</f>
+        <v>4106.1019088042485</v>
+      </c>
+      <c r="J60" s="1">
+        <f t="shared" si="11"/>
+        <v>4176.7825226190616</v>
+      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
@@ -6300,6 +6420,18 @@
       <c r="G61" s="1">
         <f t="shared" si="10"/>
         <v>69.286000000000001</v>
+      </c>
+      <c r="H61" s="1">
+        <f>F61/60000/2</f>
+        <v>3.4933303103448263E-2</v>
+      </c>
+      <c r="I61" s="1">
+        <f>F61-H61*1024</f>
+        <v>4156.2246700358601</v>
+      </c>
+      <c r="J61" s="1">
+        <f t="shared" si="11"/>
+        <v>4227.7680747917229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clicking routine works. Added dir with the roughsols for the orders not included on the old solution.
</commit_message>
<xml_diff>
--- a/OrderInfo.xlsx
+++ b/OrderInfo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Order #</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Spec Order</t>
+  </si>
+  <si>
+    <t>Auto Done</t>
   </si>
 </sst>
 </file>
@@ -630,11 +633,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1734842560"/>
-        <c:axId val="-1734837760"/>
+        <c:axId val="940720656"/>
+        <c:axId val="940725456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1734842560"/>
+        <c:axId val="940720656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -691,12 +694,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734837760"/>
+        <c:crossAx val="940725456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1734837760"/>
+        <c:axId val="940725456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -754,7 +757,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734842560"/>
+        <c:crossAx val="940720656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1315,11 +1318,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1734756752"/>
-        <c:axId val="-1734751952"/>
+        <c:axId val="940758336"/>
+        <c:axId val="940763136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1734756752"/>
+        <c:axId val="940758336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1375,12 +1378,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734751952"/>
+        <c:crossAx val="940763136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1734751952"/>
+        <c:axId val="940763136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60.0"/>
@@ -1437,7 +1440,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734756752"/>
+        <c:crossAx val="940758336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1910,11 +1913,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1734714528"/>
-        <c:axId val="-1734709728"/>
+        <c:axId val="922088880"/>
+        <c:axId val="922093648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1734714528"/>
+        <c:axId val="922088880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1970,12 +1973,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734709728"/>
+        <c:crossAx val="922093648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1734709728"/>
+        <c:axId val="922093648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -2034,7 +2037,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734714528"/>
+        <c:crossAx val="922088880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4111,8 +4114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6003,35 +6006,35 @@
       </c>
       <c r="C51" s="1">
         <f t="shared" ref="C51:C59" si="6">F52/(F52-F51)</f>
-        <v>91.920903954803137</v>
+        <v>92.089397089396101</v>
       </c>
       <c r="D51" s="1">
         <f>F51-G51/2</f>
-        <v>3704.9660138291279</v>
+        <v>3706.2633385822292</v>
       </c>
       <c r="E51" s="1">
         <f>F51+G51/2</f>
-        <v>3766.9390138291278</v>
+        <v>3768.2363385822291</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" ref="F51:F59" si="7">C52*F52/(C52+1)</f>
-        <v>3735.9525138291278</v>
+        <v>3737.2498385822291</v>
       </c>
       <c r="G51" s="1">
         <f>0.000007*A51^4-0.0004*A51^3+0.0185*A51^2+0.5793*A51+61.973</f>
         <v>61.972999999999999</v>
       </c>
       <c r="H51" s="1">
-        <f>F51/60000/2</f>
-        <v>3.1132937615242731E-2</v>
+        <f t="shared" ref="H51:H61" si="8">F51/60000/2</f>
+        <v>3.1143748654851911E-2</v>
       </c>
       <c r="I51" s="1">
-        <f>F51-H51*1024</f>
-        <v>3704.0723857111193</v>
+        <f t="shared" ref="I51:I61" si="9">F51-H51*1024</f>
+        <v>3705.3586399596606</v>
       </c>
       <c r="J51" s="1">
         <f>F51+H51*1024</f>
-        <v>3767.8326419471364</v>
+        <v>3769.1410372047976</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -6043,35 +6046,35 @@
       </c>
       <c r="C52" s="1">
         <f t="shared" si="6"/>
-        <v>90.920903954802228</v>
+        <v>91.089397089395902</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" ref="D52:D61" si="8">F52-G52/2</f>
-        <v>3745.7574485847513</v>
+        <f t="shared" ref="D52:D60" si="10">F52-G52/2</f>
+        <v>3746.9930089435079</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" ref="E52:E61" si="9">F52+G52/2</f>
-        <v>3808.3278555847514</v>
+        <f t="shared" ref="E52:E60" si="11">F52+G52/2</f>
+        <v>3809.5634159435081</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="7"/>
-        <v>3777.0426520847514</v>
+        <v>3778.278212443508</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" ref="G52:G61" si="10">0.000007*A52^4-0.0004*A52^3+0.0185*A52^2+0.5793*A52+61.973</f>
+        <f t="shared" ref="G52:G61" si="12">0.000007*A52^4-0.0004*A52^3+0.0185*A52^2+0.5793*A52+61.973</f>
         <v>62.570406999999996</v>
       </c>
       <c r="H52" s="1">
-        <f>F52/60000/2</f>
-        <v>3.1475355434039592E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.1485651770362569E-2</v>
       </c>
       <c r="I52" s="1">
-        <f>F52-H52*1024</f>
-        <v>3744.811888120295</v>
+        <f t="shared" si="9"/>
+        <v>3746.0369050306567</v>
       </c>
       <c r="J52" s="1">
-        <f t="shared" ref="J52:J61" si="11">F52+H52*1024</f>
-        <v>3809.2734160492078</v>
+        <f t="shared" ref="J52:J61" si="13">F52+H52*1024</f>
+        <v>3810.5195198563592</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -6083,35 +6086,35 @@
       </c>
       <c r="C53" s="1">
         <f t="shared" si="6"/>
-        <v>89.92090395480156</v>
+        <v>90.089397089395902</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="8"/>
-        <v>3787.4454517155004</v>
+        <f t="shared" si="10"/>
+        <v>3788.6161672109452</v>
       </c>
       <c r="E53" s="1">
-        <f t="shared" si="9"/>
-        <v>3850.6479637155003</v>
+        <f t="shared" si="11"/>
+        <v>3851.818679210945</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="7"/>
-        <v>3819.0467077155004</v>
+        <v>3820.2174232109451</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>63.202511999999999</v>
       </c>
       <c r="H53" s="1">
-        <f>F53/60000/2</f>
-        <v>3.1825389230962502E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.1835145193424542E-2</v>
       </c>
       <c r="I53" s="1">
-        <f>F53-H53*1024</f>
-        <v>3786.4575091429947</v>
+        <f t="shared" si="9"/>
+        <v>3787.6182345328784</v>
       </c>
       <c r="J53" s="1">
-        <f t="shared" si="11"/>
-        <v>3851.635906288006</v>
+        <f t="shared" si="13"/>
+        <v>3852.8166118890117</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -6123,35 +6126,35 @@
       </c>
       <c r="C54" s="1">
         <f t="shared" si="6"/>
-        <v>88.920903954801304</v>
+        <v>89.089397089396002</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="8"/>
-        <v>3830.0619308274609</v>
+        <f t="shared" si="10"/>
+        <v>3831.1645589437576</v>
       </c>
       <c r="E54" s="1">
-        <f t="shared" si="9"/>
-        <v>3893.9290978274612</v>
+        <f t="shared" si="11"/>
+        <v>3895.0317259437579</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="7"/>
-        <v>3861.995514327461</v>
+        <v>3863.0981424437578</v>
       </c>
       <c r="G54" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>63.867167000000002</v>
       </c>
       <c r="H54" s="1">
-        <f>F54/60000/2</f>
-        <v>3.2183295952728841E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.2192484520364648E-2</v>
       </c>
       <c r="I54" s="1">
-        <f>F54-H54*1024</f>
-        <v>3829.0398192718667</v>
+        <f t="shared" si="9"/>
+        <v>3830.1330382949045</v>
       </c>
       <c r="J54" s="1">
-        <f t="shared" si="11"/>
-        <v>3894.9512093830554</v>
+        <f t="shared" si="13"/>
+        <v>3896.063246592611</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -6163,35 +6166,35 @@
       </c>
       <c r="C55" s="1">
         <f t="shared" si="6"/>
-        <v>87.920903954800934</v>
+        <v>88.089397089396002</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="8"/>
-        <v>3873.6401123151213</v>
+        <f t="shared" si="10"/>
+        <v>3874.6712384480879</v>
       </c>
       <c r="E55" s="1">
-        <f t="shared" si="9"/>
-        <v>3938.2025043151211</v>
+        <f t="shared" si="11"/>
+        <v>3939.2336304480878</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="7"/>
-        <v>3905.9213083151212</v>
+        <v>3906.9524344480878</v>
       </c>
       <c r="G55" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>64.562392000000003</v>
       </c>
       <c r="H55" s="1">
-        <f>F55/60000/2</f>
-        <v>3.2549344235959343E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.2557936953734067E-2</v>
       </c>
       <c r="I55" s="1">
-        <f>F55-H55*1024</f>
-        <v>3872.590779817499</v>
+        <f t="shared" si="9"/>
+        <v>3873.6131070074644</v>
       </c>
       <c r="J55" s="1">
-        <f t="shared" si="11"/>
-        <v>3939.2518368127435</v>
+        <f t="shared" si="13"/>
+        <v>3940.2917618887113</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -6203,35 +6206,35 @@
       </c>
       <c r="C56" s="1">
         <f t="shared" si="6"/>
-        <v>86.92090395480119</v>
+        <v>87.08939708939603</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="8"/>
-        <v>3918.2146220547565</v>
+        <f t="shared" si="10"/>
+        <v>3919.1706487377646</v>
       </c>
       <c r="E56" s="1">
-        <f t="shared" si="9"/>
-        <v>3983.5009970547562</v>
+        <f t="shared" si="11"/>
+        <v>3984.4570237377643</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="7"/>
-        <v>3950.8578095547564</v>
+        <v>3951.8138362377645</v>
       </c>
       <c r="G56" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>65.286374999999992</v>
       </c>
       <c r="H56" s="1">
-        <f>F56/60000/2</f>
-        <v>3.292381507962297E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.2931781968648037E-2</v>
       </c>
       <c r="I56" s="1">
-        <f>F56-H56*1024</f>
-        <v>3917.1438229132223</v>
+        <f t="shared" si="9"/>
+        <v>3918.0916915018688</v>
       </c>
       <c r="J56" s="1">
-        <f t="shared" si="11"/>
-        <v>3984.5717961962905</v>
+        <f t="shared" si="13"/>
+        <v>3985.5359809736601</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -6243,35 +6246,35 @@
       </c>
       <c r="C57" s="1">
         <f t="shared" si="6"/>
-        <v>85.920903954801702</v>
+        <v>86.089397089396385</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="8"/>
-        <v>3963.821571732768</v>
+        <f t="shared" si="10"/>
+        <v>3964.6987070679315</v>
       </c>
       <c r="E57" s="1">
-        <f t="shared" si="9"/>
-        <v>4029.859043732768</v>
+        <f t="shared" si="11"/>
+        <v>4030.7361790679315</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="7"/>
-        <v>3996.840307732768</v>
+        <v>3997.7174430679315</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>66.037471999999994</v>
       </c>
       <c r="H57" s="1">
-        <f>F57/60000/2</f>
-        <v>3.3307002564439733E-2</v>
+        <f t="shared" si="8"/>
+        <v>3.3314312025566097E-2</v>
       </c>
       <c r="I57" s="1">
-        <f>F57-H57*1024</f>
-        <v>3962.7339371067819</v>
+        <f t="shared" si="9"/>
+        <v>3963.6035875537518</v>
       </c>
       <c r="J57" s="1">
-        <f t="shared" si="11"/>
-        <v>4030.9466783587541</v>
+        <f t="shared" si="13"/>
+        <v>4031.8312985821112</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -6283,35 +6286,35 @@
       </c>
       <c r="C58" s="1">
         <f t="shared" si="6"/>
-        <v>84.920903954801361</v>
+        <v>85.089397089396456</v>
       </c>
       <c r="D58" s="1">
+        <v>4010.5</v>
+      </c>
+      <c r="E58" s="1">
+        <v>4077.5</v>
+      </c>
+      <c r="F58" s="1">
+        <v>4044.7</v>
+      </c>
+      <c r="G58" s="1">
+        <f>E58-D58</f>
+        <v>67</v>
+      </c>
+      <c r="H58" s="1">
         <f t="shared" si="8"/>
-        <v>4010.498651273464</v>
-      </c>
-      <c r="E58" s="1">
+        <v>3.3705833333333331E-2</v>
+      </c>
+      <c r="I58" s="1">
         <f t="shared" si="9"/>
-        <v>4077.3128582734644</v>
-      </c>
-      <c r="F58" s="1">
-        <f t="shared" si="7"/>
-        <v>4043.9057547734642</v>
-      </c>
-      <c r="G58" s="1">
-        <f t="shared" si="10"/>
-        <v>66.814206999999996</v>
-      </c>
-      <c r="H58" s="1">
-        <f>F58/60000/2</f>
-        <v>3.3699214623112199E-2</v>
-      </c>
-      <c r="I58" s="1">
-        <f>F58-H58*1024</f>
-        <v>4009.3977589993974</v>
+        <v>4010.1852266666665</v>
       </c>
       <c r="J58" s="1">
-        <f t="shared" si="11"/>
-        <v>4078.413750547531</v>
+        <f t="shared" si="13"/>
+        <v>4079.2147733333331</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -6323,35 +6326,35 @@
       </c>
       <c r="C59" s="1">
         <f t="shared" si="6"/>
-        <v>83.920903954800693</v>
+        <v>83.850202429150414</v>
       </c>
       <c r="D59" s="1">
+        <v>4058.3</v>
+      </c>
+      <c r="E59" s="1">
+        <v>4126.1000000000004</v>
+      </c>
+      <c r="F59" s="1">
+        <v>4092.8</v>
+      </c>
+      <c r="G59" s="1">
+        <f>E59-D59</f>
+        <v>67.800000000000182</v>
+      </c>
+      <c r="H59" s="1">
         <f t="shared" si="8"/>
-        <v>4058.285227875047</v>
-      </c>
-      <c r="E59" s="1">
+        <v>3.4106666666666667E-2</v>
+      </c>
+      <c r="I59" s="1">
         <f t="shared" si="9"/>
-        <v>4125.900499875047</v>
-      </c>
-      <c r="F59" s="1">
-        <f t="shared" si="7"/>
-        <v>4092.092863875047</v>
-      </c>
-      <c r="G59" s="1">
-        <f t="shared" si="10"/>
-        <v>67.615272000000004</v>
-      </c>
-      <c r="H59" s="1">
-        <f>F59/60000/2</f>
-        <v>3.4100773865625392E-2</v>
-      </c>
-      <c r="I59" s="1">
-        <f>F59-H59*1024</f>
-        <v>4057.1736714366466</v>
+        <v>4057.8747733333335</v>
       </c>
       <c r="J59" s="1">
-        <f t="shared" si="11"/>
-        <v>4127.0120563134478</v>
+        <f t="shared" si="13"/>
+        <v>4127.7252266666665</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -6363,35 +6366,35 @@
       </c>
       <c r="C60" s="1">
         <f>F61/(F61-F60)</f>
-        <v>82.920903954800565</v>
+        <v>83.023762376237613</v>
       </c>
       <c r="D60" s="1">
+        <v>4107.2</v>
+      </c>
+      <c r="E60" s="1">
+        <v>4175.8</v>
+      </c>
+      <c r="F60" s="1">
+        <v>4142.2</v>
+      </c>
+      <c r="G60" s="1">
+        <f>E60-D60</f>
+        <v>68.600000000000364</v>
+      </c>
+      <c r="H60" s="1">
         <f t="shared" si="8"/>
-        <v>4107.2224522116549</v>
-      </c>
-      <c r="E60" s="1">
+        <v>3.4518333333333331E-2</v>
+      </c>
+      <c r="I60" s="1">
         <f t="shared" si="9"/>
-        <v>4175.6619792116553</v>
-      </c>
-      <c r="F60" s="1">
-        <f>C61*F61/(C61+1)</f>
-        <v>4141.4422157116551</v>
-      </c>
-      <c r="G60" s="1">
-        <f t="shared" si="10"/>
-        <v>68.439526999999998</v>
-      </c>
-      <c r="H60" s="1">
-        <f>F60/60000/2</f>
-        <v>3.4512018464263793E-2</v>
-      </c>
-      <c r="I60" s="1">
-        <f>F60-H60*1024</f>
-        <v>4106.1019088042485</v>
+        <v>4106.8532266666662</v>
       </c>
       <c r="J60" s="1">
-        <f t="shared" si="11"/>
-        <v>4176.7825226190616</v>
+        <f t="shared" si="13"/>
+        <v>4177.5467733333335</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -6403,35 +6406,35 @@
       </c>
       <c r="C61" s="1">
         <f>F2/(F2-F61)</f>
-        <v>81.920903954800863</v>
+        <v>83.048923679061545</v>
       </c>
       <c r="D61" s="1">
+        <v>4157.3</v>
+      </c>
+      <c r="E61" s="1">
+        <v>4226.7</v>
+      </c>
+      <c r="F61" s="1">
+        <v>4192.7</v>
+      </c>
+      <c r="G61" s="1">
+        <f>E61-D61</f>
+        <v>69.399999999999636</v>
+      </c>
+      <c r="H61" s="1">
         <f t="shared" si="8"/>
-        <v>4157.3533724137915</v>
-      </c>
-      <c r="E61" s="1">
+        <v>3.4939166666666667E-2</v>
+      </c>
+      <c r="I61" s="1">
         <f t="shared" si="9"/>
-        <v>4226.6393724137915</v>
-      </c>
-      <c r="F61" s="1">
-        <f>C2*F2/(C2+1)</f>
-        <v>4191.9963724137915</v>
-      </c>
-      <c r="G61" s="1">
-        <f t="shared" si="10"/>
-        <v>69.286000000000001</v>
-      </c>
-      <c r="H61" s="1">
-        <f>F61/60000/2</f>
-        <v>3.4933303103448263E-2</v>
-      </c>
-      <c r="I61" s="1">
-        <f>F61-H61*1024</f>
-        <v>4156.2246700358601</v>
+        <v>4156.9222933333331</v>
       </c>
       <c r="J61" s="1">
-        <f t="shared" si="11"/>
-        <v>4227.7680747917229</v>
+        <f t="shared" si="13"/>
+        <v>4228.4777066666666</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Did two more orders, 6 and 5.
</commit_message>
<xml_diff>
--- a/OrderInfo.xlsx
+++ b/OrderInfo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Order #</t>
   </si>
@@ -4115,7 +4115,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6006,19 +6006,19 @@
       </c>
       <c r="C51" s="1">
         <f t="shared" ref="C51:C59" si="6">F52/(F52-F51)</f>
-        <v>92.089397089396101</v>
+        <v>91.904347826086934</v>
       </c>
       <c r="D51" s="1">
         <f>F51-G51/2</f>
-        <v>3706.2633385822292</v>
+        <v>3705.6291116945781</v>
       </c>
       <c r="E51" s="1">
         <f>F51+G51/2</f>
-        <v>3768.2363385822291</v>
+        <v>3767.6021116945781</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" ref="F51:F59" si="7">C52*F52/(C52+1)</f>
-        <v>3737.2498385822291</v>
+        <v>3736.6156116945781</v>
       </c>
       <c r="G51" s="1">
         <f>0.000007*A51^4-0.0004*A51^3+0.0185*A51^2+0.5793*A51+61.973</f>
@@ -6026,15 +6026,15 @@
       </c>
       <c r="H51" s="1">
         <f t="shared" ref="H51:H61" si="8">F51/60000/2</f>
-        <v>3.1143748654851911E-2</v>
+        <v>3.113846343078815E-2</v>
       </c>
       <c r="I51" s="1">
         <f t="shared" ref="I51:I61" si="9">F51-H51*1024</f>
-        <v>3705.3586399596606</v>
+        <v>3704.7298251414509</v>
       </c>
       <c r="J51" s="1">
         <f>F51+H51*1024</f>
-        <v>3769.1410372047976</v>
+        <v>3768.5013982477053</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -6046,19 +6046,19 @@
       </c>
       <c r="C52" s="1">
         <f t="shared" si="6"/>
-        <v>91.089397089395902</v>
+        <v>90.904347826087303</v>
       </c>
       <c r="D52" s="1">
         <f t="shared" ref="D52:D60" si="10">F52-G52/2</f>
-        <v>3746.9930089435079</v>
+        <v>3746.4353245275488</v>
       </c>
       <c r="E52" s="1">
         <f t="shared" ref="E52:E60" si="11">F52+G52/2</f>
-        <v>3809.5634159435081</v>
+        <v>3809.005731527549</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="7"/>
-        <v>3778.278212443508</v>
+        <v>3777.7205280275489</v>
       </c>
       <c r="G52" s="1">
         <f t="shared" ref="G52:G61" si="12">0.000007*A52^4-0.0004*A52^3+0.0185*A52^2+0.5793*A52+61.973</f>
@@ -6066,15 +6066,15 @@
       </c>
       <c r="H52" s="1">
         <f t="shared" si="8"/>
-        <v>3.1485651770362569E-2</v>
+        <v>3.1481004400229572E-2</v>
       </c>
       <c r="I52" s="1">
         <f t="shared" si="9"/>
-        <v>3746.0369050306567</v>
+        <v>3745.483979521714</v>
       </c>
       <c r="J52" s="1">
         <f t="shared" ref="J52:J61" si="13">F52+H52*1024</f>
-        <v>3810.5195198563592</v>
+        <v>3809.9570765333838</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -6086,19 +6086,19 @@
       </c>
       <c r="C53" s="1">
         <f t="shared" si="6"/>
-        <v>90.089397089395902</v>
+        <v>89.904347826086948</v>
       </c>
       <c r="D53" s="1">
         <f t="shared" si="10"/>
-        <v>3788.6161672109452</v>
+        <v>3788.1386027871163</v>
       </c>
       <c r="E53" s="1">
         <f t="shared" si="11"/>
-        <v>3851.818679210945</v>
+        <v>3851.3411147871161</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="7"/>
-        <v>3820.2174232109451</v>
+        <v>3819.7398587871162</v>
       </c>
       <c r="G53" s="1">
         <f t="shared" si="12"/>
@@ -6106,15 +6106,15 @@
       </c>
       <c r="H53" s="1">
         <f t="shared" si="8"/>
-        <v>3.1835145193424542E-2</v>
+        <v>3.1831165489892635E-2</v>
       </c>
       <c r="I53" s="1">
         <f t="shared" si="9"/>
-        <v>3787.6182345328784</v>
+        <v>3787.1447453254659</v>
       </c>
       <c r="J53" s="1">
         <f t="shared" si="13"/>
-        <v>3852.8166118890117</v>
+        <v>3852.3349722487665</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -6126,19 +6126,19 @@
       </c>
       <c r="C54" s="1">
         <f t="shared" si="6"/>
-        <v>89.089397089396002</v>
+        <v>88.904347826086621</v>
       </c>
       <c r="D54" s="1">
         <f t="shared" si="10"/>
-        <v>3831.1645589437576</v>
+        <v>3830.770876593896</v>
       </c>
       <c r="E54" s="1">
         <f t="shared" si="11"/>
-        <v>3895.0317259437579</v>
+        <v>3894.6380435938963</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="7"/>
-        <v>3863.0981424437578</v>
+        <v>3862.7044600938962</v>
       </c>
       <c r="G54" s="1">
         <f t="shared" si="12"/>
@@ -6146,15 +6146,15 @@
       </c>
       <c r="H54" s="1">
         <f t="shared" si="8"/>
-        <v>3.2192484520364648E-2</v>
+        <v>3.2189203834115804E-2</v>
       </c>
       <c r="I54" s="1">
         <f t="shared" si="9"/>
-        <v>3830.1330382949045</v>
+        <v>3829.7427153677618</v>
       </c>
       <c r="J54" s="1">
         <f t="shared" si="13"/>
-        <v>3896.063246592611</v>
+        <v>3895.6662048200305</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -6166,19 +6166,19 @@
       </c>
       <c r="C55" s="1">
         <f t="shared" si="6"/>
-        <v>88.089397089396002</v>
+        <v>87.904347826086365</v>
       </c>
       <c r="D55" s="1">
         <f t="shared" si="10"/>
-        <v>3874.6712384480879</v>
+        <v>3874.3653961456125</v>
       </c>
       <c r="E55" s="1">
         <f t="shared" si="11"/>
-        <v>3939.2336304480878</v>
+        <v>3938.9277881456123</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="7"/>
-        <v>3906.9524344480878</v>
+        <v>3906.6465921456124</v>
       </c>
       <c r="G55" s="1">
         <f t="shared" si="12"/>
@@ -6186,15 +6186,15 @@
       </c>
       <c r="H55" s="1">
         <f t="shared" si="8"/>
-        <v>3.2557936953734067E-2</v>
+        <v>3.2555388267880105E-2</v>
       </c>
       <c r="I55" s="1">
         <f t="shared" si="9"/>
-        <v>3873.6131070074644</v>
+        <v>3873.3098745593034</v>
       </c>
       <c r="J55" s="1">
         <f t="shared" si="13"/>
-        <v>3940.2917618887113</v>
+        <v>3939.9833097319215</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -6206,35 +6206,35 @@
       </c>
       <c r="C56" s="1">
         <f t="shared" si="6"/>
-        <v>87.08939708939603</v>
+        <v>86.904347826086948</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="10"/>
-        <v>3919.1706487377646</v>
+        <v>3918.2</v>
       </c>
       <c r="E56" s="1">
-        <f t="shared" si="11"/>
-        <v>3984.4570237377643</v>
+        <v>3983.7</v>
       </c>
       <c r="F56" s="1">
-        <f t="shared" si="7"/>
-        <v>3951.8138362377645</v>
+        <v>3951.6</v>
       </c>
       <c r="G56" s="1">
-        <f t="shared" si="12"/>
-        <v>65.286374999999992</v>
+        <f>E56-D56</f>
+        <v>65.5</v>
       </c>
       <c r="H56" s="1">
         <f t="shared" si="8"/>
-        <v>3.2931781968648037E-2</v>
+        <v>3.2930000000000001E-2</v>
       </c>
       <c r="I56" s="1">
         <f t="shared" si="9"/>
-        <v>3918.0916915018688</v>
+        <v>3917.87968</v>
       </c>
       <c r="J56" s="1">
         <f t="shared" si="13"/>
-        <v>3985.5359809736601</v>
+        <v>3985.3203199999998</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -6246,35 +6246,35 @@
       </c>
       <c r="C57" s="1">
         <f t="shared" si="6"/>
-        <v>86.089397089396385</v>
+        <v>85.874734607218841</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="10"/>
-        <v>3964.6987070679315</v>
+        <v>3963.9</v>
       </c>
       <c r="E57" s="1">
-        <f t="shared" si="11"/>
-        <v>4030.7361790679315</v>
+        <v>4030.1</v>
       </c>
       <c r="F57" s="1">
-        <f t="shared" si="7"/>
-        <v>3997.7174430679315</v>
+        <v>3997.6</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" si="12"/>
-        <v>66.037471999999994</v>
+        <f>E57-D57</f>
+        <v>66.199999999999818</v>
       </c>
       <c r="H57" s="1">
         <f t="shared" si="8"/>
-        <v>3.3314312025566097E-2</v>
+        <v>3.3313333333333334E-2</v>
       </c>
       <c r="I57" s="1">
         <f t="shared" si="9"/>
-        <v>3963.6035875537518</v>
+        <v>3963.4871466666664</v>
       </c>
       <c r="J57" s="1">
         <f t="shared" si="13"/>
-        <v>4031.8312985821112</v>
+        <v>4031.7128533333334</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Did another order: #4
</commit_message>
<xml_diff>
--- a/OrderInfo.xlsx
+++ b/OrderInfo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmk2347/codes/coudereduction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boydrummer94/Research/Codes/coudereduction/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>Order #</t>
   </si>
@@ -253,7 +253,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -633,11 +632,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="940720656"/>
-        <c:axId val="940725456"/>
+        <c:axId val="227799872"/>
+        <c:axId val="227804672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="940720656"/>
+        <c:axId val="227799872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,12 +693,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="940725456"/>
+        <c:crossAx val="227804672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="940725456"/>
+        <c:axId val="227804672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -757,7 +756,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="940720656"/>
+        <c:crossAx val="227799872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1318,11 +1317,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="940758336"/>
-        <c:axId val="940763136"/>
+        <c:axId val="227902608"/>
+        <c:axId val="227907408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="940758336"/>
+        <c:axId val="227902608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1378,12 +1377,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="940763136"/>
+        <c:crossAx val="227907408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="940763136"/>
+        <c:axId val="227907408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60.0"/>
@@ -1440,7 +1439,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="940758336"/>
+        <c:crossAx val="227902608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1533,7 +1532,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1913,11 +1911,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="922088880"/>
-        <c:axId val="922093648"/>
+        <c:axId val="227952496"/>
+        <c:axId val="227957296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="922088880"/>
+        <c:axId val="227952496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1973,12 +1971,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="922093648"/>
+        <c:crossAx val="227957296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="922093648"/>
+        <c:axId val="227957296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -2037,7 +2035,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="922088880"/>
+        <c:crossAx val="227952496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4114,8 +4112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6006,19 +6004,19 @@
       </c>
       <c r="C51" s="1">
         <f t="shared" ref="C51:C59" si="6">F52/(F52-F51)</f>
-        <v>91.904347826086934</v>
+        <v>92.008908685968507</v>
       </c>
       <c r="D51" s="1">
         <f>F51-G51/2</f>
-        <v>3705.6291116945781</v>
+        <v>3705.873424477149</v>
       </c>
       <c r="E51" s="1">
         <f>F51+G51/2</f>
-        <v>3767.6021116945781</v>
+        <v>3767.846424477149</v>
       </c>
       <c r="F51" s="1">
-        <f t="shared" ref="F51:F59" si="7">C52*F52/(C52+1)</f>
-        <v>3736.6156116945781</v>
+        <f t="shared" ref="F51:F55" si="7">C52*F52/(C52+1)</f>
+        <v>3736.859924477149</v>
       </c>
       <c r="G51" s="1">
         <f>0.000007*A51^4-0.0004*A51^3+0.0185*A51^2+0.5793*A51+61.973</f>
@@ -6026,15 +6024,15 @@
       </c>
       <c r="H51" s="1">
         <f t="shared" ref="H51:H61" si="8">F51/60000/2</f>
-        <v>3.113846343078815E-2</v>
+        <v>3.1140499370642907E-2</v>
       </c>
       <c r="I51" s="1">
         <f t="shared" ref="I51:I61" si="9">F51-H51*1024</f>
-        <v>3704.7298251414509</v>
+        <v>3704.9720531216108</v>
       </c>
       <c r="J51" s="1">
         <f>F51+H51*1024</f>
-        <v>3768.5013982477053</v>
+        <v>3768.7477958326872</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -6046,35 +6044,35 @@
       </c>
       <c r="C52" s="1">
         <f t="shared" si="6"/>
-        <v>90.904347826087303</v>
+        <v>91.008908685968464</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" ref="D52:D60" si="10">F52-G52/2</f>
-        <v>3746.4353245275488</v>
+        <f t="shared" ref="D52:D55" si="10">F52-G52/2</f>
+        <v>3746.6350960374784</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" ref="E52:E60" si="11">F52+G52/2</f>
-        <v>3809.005731527549</v>
+        <f t="shared" ref="E52:E55" si="11">F52+G52/2</f>
+        <v>3809.2055030374786</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="7"/>
-        <v>3777.7205280275489</v>
+        <v>3777.9202995374785</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" ref="G52:G61" si="12">0.000007*A52^4-0.0004*A52^3+0.0185*A52^2+0.5793*A52+61.973</f>
+        <f t="shared" ref="G52:G55" si="12">0.000007*A52^4-0.0004*A52^3+0.0185*A52^2+0.5793*A52+61.973</f>
         <v>62.570406999999996</v>
       </c>
       <c r="H52" s="1">
         <f t="shared" si="8"/>
-        <v>3.1481004400229572E-2</v>
+        <v>3.1482669162812324E-2</v>
       </c>
       <c r="I52" s="1">
         <f t="shared" si="9"/>
-        <v>3745.483979521714</v>
+        <v>3745.6820463147587</v>
       </c>
       <c r="J52" s="1">
         <f t="shared" ref="J52:J61" si="13">F52+H52*1024</f>
-        <v>3809.9570765333838</v>
+        <v>3810.1585527601983</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -6086,19 +6084,19 @@
       </c>
       <c r="C53" s="1">
         <f t="shared" si="6"/>
-        <v>89.904347826086948</v>
+        <v>90.008908685968649</v>
       </c>
       <c r="D53" s="1">
         <f t="shared" si="10"/>
-        <v>3788.1386027871163</v>
+        <v>3788.291781066363</v>
       </c>
       <c r="E53" s="1">
         <f t="shared" si="11"/>
-        <v>3851.3411147871161</v>
+        <v>3851.4942930663628</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="7"/>
-        <v>3819.7398587871162</v>
+        <v>3819.8930370663629</v>
       </c>
       <c r="G53" s="1">
         <f t="shared" si="12"/>
@@ -6106,15 +6104,15 @@
       </c>
       <c r="H53" s="1">
         <f t="shared" si="8"/>
-        <v>3.1831165489892635E-2</v>
+        <v>3.1832441975553023E-2</v>
       </c>
       <c r="I53" s="1">
         <f t="shared" si="9"/>
-        <v>3787.1447453254659</v>
+        <v>3787.2966164833965</v>
       </c>
       <c r="J53" s="1">
         <f t="shared" si="13"/>
-        <v>3852.3349722487665</v>
+        <v>3852.4894576493293</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -6126,19 +6124,19 @@
       </c>
       <c r="C54" s="1">
         <f t="shared" si="6"/>
-        <v>88.904347826086621</v>
+        <v>89.008908685968905</v>
       </c>
       <c r="D54" s="1">
         <f t="shared" si="10"/>
-        <v>3830.770876593896</v>
+        <v>3830.8753042768044</v>
       </c>
       <c r="E54" s="1">
         <f t="shared" si="11"/>
-        <v>3894.6380435938963</v>
+        <v>3894.7424712768047</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="7"/>
-        <v>3862.7044600938962</v>
+        <v>3862.8088877768046</v>
       </c>
       <c r="G54" s="1">
         <f t="shared" si="12"/>
@@ -6146,15 +6144,15 @@
       </c>
       <c r="H54" s="1">
         <f t="shared" si="8"/>
-        <v>3.2189203834115804E-2</v>
+        <v>3.2190074064806708E-2</v>
       </c>
       <c r="I54" s="1">
         <f t="shared" si="9"/>
-        <v>3829.7427153677618</v>
+        <v>3829.8462519344425</v>
       </c>
       <c r="J54" s="1">
         <f t="shared" si="13"/>
-        <v>3895.6662048200305</v>
+        <v>3895.7715236191666</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -6166,35 +6164,35 @@
       </c>
       <c r="C55" s="1">
         <f t="shared" si="6"/>
-        <v>87.904347826086365</v>
+        <v>88.008908685968635</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="10"/>
-        <v>3874.3653961456125</v>
+        <v>3874.2</v>
       </c>
       <c r="E55" s="1">
-        <f t="shared" si="11"/>
-        <v>3938.9277881456123</v>
+        <v>3938.7</v>
       </c>
       <c r="F55" s="1">
-        <f t="shared" si="7"/>
-        <v>3906.6465921456124</v>
+        <v>3906.7</v>
       </c>
       <c r="G55" s="1">
-        <f t="shared" si="12"/>
-        <v>64.562392000000003</v>
+        <f>E55-D55</f>
+        <v>64.5</v>
       </c>
       <c r="H55" s="1">
         <f t="shared" si="8"/>
-        <v>3.2555388267880105E-2</v>
+        <v>3.2555833333333332E-2</v>
       </c>
       <c r="I55" s="1">
         <f t="shared" si="9"/>
-        <v>3873.3098745593034</v>
+        <v>3873.3628266666665</v>
       </c>
       <c r="J55" s="1">
         <f t="shared" si="13"/>
-        <v>3939.9833097319215</v>
+        <v>3940.0371733333332</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -6218,7 +6216,7 @@
         <v>3951.6</v>
       </c>
       <c r="G56" s="1">
-        <f>E56-D56</f>
+        <f t="shared" ref="G56:G61" si="14">E56-D56</f>
         <v>65.5</v>
       </c>
       <c r="H56" s="1">
@@ -6258,7 +6256,7 @@
         <v>3997.6</v>
       </c>
       <c r="G57" s="1">
-        <f>E57-D57</f>
+        <f t="shared" si="14"/>
         <v>66.199999999999818</v>
       </c>
       <c r="H57" s="1">
@@ -6298,7 +6296,7 @@
         <v>4044.7</v>
       </c>
       <c r="G58" s="1">
-        <f>E58-D58</f>
+        <f t="shared" si="14"/>
         <v>67</v>
       </c>
       <c r="H58" s="1">
@@ -6338,7 +6336,7 @@
         <v>4092.8</v>
       </c>
       <c r="G59" s="1">
-        <f>E59-D59</f>
+        <f t="shared" si="14"/>
         <v>67.800000000000182</v>
       </c>
       <c r="H59" s="1">
@@ -6378,7 +6376,7 @@
         <v>4142.2</v>
       </c>
       <c r="G60" s="1">
-        <f>E60-D60</f>
+        <f t="shared" si="14"/>
         <v>68.600000000000364</v>
       </c>
       <c r="H60" s="1">
@@ -6418,7 +6416,7 @@
         <v>4192.7</v>
       </c>
       <c r="G61" s="1">
-        <f>E61-D61</f>
+        <f t="shared" si="14"/>
         <v>69.399999999999636</v>
       </c>
       <c r="H61" s="1">

</xml_diff>

<commit_message>
Finished the manual solutions for the orders that needed it. The one order with a previous sol -- 58 -- is still weird. Just not many lines. Hm
</commit_message>
<xml_diff>
--- a/OrderInfo.xlsx
+++ b/OrderInfo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boydrummer94/Research/Codes/coudereduction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmk2347/codes/coudereduction/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Order #</t>
   </si>
@@ -632,11 +632,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="227799872"/>
-        <c:axId val="227804672"/>
+        <c:axId val="-254523840"/>
+        <c:axId val="-241247184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="227799872"/>
+        <c:axId val="-254523840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -693,12 +693,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227804672"/>
+        <c:crossAx val="-241247184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="227804672"/>
+        <c:axId val="-241247184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -756,7 +756,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227799872"/>
+        <c:crossAx val="-254523840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1317,11 +1317,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="227902608"/>
-        <c:axId val="227907408"/>
+        <c:axId val="-271333312"/>
+        <c:axId val="-251854576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="227902608"/>
+        <c:axId val="-271333312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1341,6 +1341,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1377,12 +1378,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227907408"/>
+        <c:crossAx val="-251854576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="227907408"/>
+        <c:axId val="-251854576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60.0"/>
@@ -1439,7 +1440,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227902608"/>
+        <c:crossAx val="-271333312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1911,11 +1912,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="227952496"/>
-        <c:axId val="227957296"/>
+        <c:axId val="-254299024"/>
+        <c:axId val="-258067952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="227952496"/>
+        <c:axId val="-254299024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1971,12 +1972,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227957296"/>
+        <c:crossAx val="-258067952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="227957296"/>
+        <c:axId val="-258067952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -2035,7 +2036,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227952496"/>
+        <c:crossAx val="-254299024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4113,7 +4114,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="K55" sqref="K55"/>
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6004,35 +6005,35 @@
       </c>
       <c r="C51" s="1">
         <f t="shared" ref="C51:C59" si="6">F52/(F52-F51)</f>
-        <v>92.008908685968507</v>
+        <v>91.917274939171946</v>
       </c>
       <c r="D51" s="1">
-        <f>F51-G51/2</f>
-        <v>3705.873424477149</v>
+        <v>3705.1</v>
       </c>
       <c r="E51" s="1">
-        <f>F51+G51/2</f>
-        <v>3767.846424477149</v>
+        <v>3767</v>
       </c>
       <c r="F51" s="1">
-        <f t="shared" ref="F51:F55" si="7">C52*F52/(C52+1)</f>
-        <v>3736.859924477149</v>
+        <v>3736.7</v>
       </c>
       <c r="G51" s="1">
-        <f>0.000007*A51^4-0.0004*A51^3+0.0185*A51^2+0.5793*A51+61.973</f>
-        <v>61.972999999999999</v>
+        <f>E51-D51</f>
+        <v>61.900000000000091</v>
       </c>
       <c r="H51" s="1">
-        <f t="shared" ref="H51:H61" si="8">F51/60000/2</f>
-        <v>3.1140499370642907E-2</v>
+        <f t="shared" ref="H51:H61" si="7">F51/60000/2</f>
+        <v>3.1139166666666666E-2</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" ref="I51:I61" si="9">F51-H51*1024</f>
-        <v>3704.9720531216108</v>
+        <f t="shared" ref="I51:I61" si="8">F51-H51*1024</f>
+        <v>3704.8134933333331</v>
       </c>
       <c r="J51" s="1">
         <f>F51+H51*1024</f>
-        <v>3768.7477958326872</v>
+        <v>3768.5865066666665</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -6044,35 +6045,35 @@
       </c>
       <c r="C52" s="1">
         <f t="shared" si="6"/>
-        <v>91.008908685968464</v>
+        <v>90.947619047619057</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" ref="D52:D55" si="10">F52-G52/2</f>
-        <v>3746.6350960374784</v>
+        <v>3746.2</v>
       </c>
       <c r="E52" s="1">
-        <f t="shared" ref="E52:E55" si="11">F52+G52/2</f>
-        <v>3809.2055030374786</v>
+        <v>3808.5</v>
       </c>
       <c r="F52" s="1">
+        <v>3777.8</v>
+      </c>
+      <c r="G52" s="1">
+        <f>E52-D52</f>
+        <v>62.300000000000182</v>
+      </c>
+      <c r="H52" s="1">
         <f t="shared" si="7"/>
-        <v>3777.9202995374785</v>
-      </c>
-      <c r="G52" s="1">
-        <f t="shared" ref="G52:G55" si="12">0.000007*A52^4-0.0004*A52^3+0.0185*A52^2+0.5793*A52+61.973</f>
-        <v>62.570406999999996</v>
-      </c>
-      <c r="H52" s="1">
+        <v>3.1481666666666665E-2</v>
+      </c>
+      <c r="I52" s="1">
         <f t="shared" si="8"/>
-        <v>3.1482669162812324E-2</v>
-      </c>
-      <c r="I52" s="1">
-        <f t="shared" si="9"/>
-        <v>3745.6820463147587</v>
+        <v>3745.5627733333336</v>
       </c>
       <c r="J52" s="1">
-        <f t="shared" ref="J52:J61" si="13">F52+H52*1024</f>
-        <v>3810.1585527601983</v>
+        <f t="shared" ref="J52:J61" si="9">F52+H52*1024</f>
+        <v>3810.0372266666668</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -6084,35 +6085,35 @@
       </c>
       <c r="C53" s="1">
         <f t="shared" si="6"/>
-        <v>90.008908685968649</v>
+        <v>89.832558139534882</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="10"/>
-        <v>3788.291781066363</v>
+        <v>3787.5</v>
       </c>
       <c r="E53" s="1">
-        <f t="shared" si="11"/>
-        <v>3851.4942930663628</v>
+        <v>3850.8</v>
       </c>
       <c r="F53" s="1">
+        <v>3819.8</v>
+      </c>
+      <c r="G53" s="1">
+        <f>E53-D53</f>
+        <v>63.300000000000182</v>
+      </c>
+      <c r="H53" s="1">
         <f t="shared" si="7"/>
-        <v>3819.8930370663629</v>
-      </c>
-      <c r="G53" s="1">
-        <f t="shared" si="12"/>
-        <v>63.202511999999999</v>
-      </c>
-      <c r="H53" s="1">
+        <v>3.1831666666666668E-2</v>
+      </c>
+      <c r="I53" s="1">
         <f t="shared" si="8"/>
-        <v>3.1832441975553023E-2</v>
-      </c>
-      <c r="I53" s="1">
+        <v>3787.2043733333335</v>
+      </c>
+      <c r="J53" s="1">
         <f t="shared" si="9"/>
-        <v>3787.2966164833965</v>
-      </c>
-      <c r="J53" s="1">
-        <f t="shared" si="13"/>
-        <v>3852.4894576493293</v>
+        <v>3852.3956266666669</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -6124,35 +6125,35 @@
       </c>
       <c r="C54" s="1">
         <f t="shared" si="6"/>
-        <v>89.008908685968905</v>
+        <v>88.990888382688667</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="10"/>
-        <v>3830.8753042768044</v>
+        <v>3830.1</v>
       </c>
       <c r="E54" s="1">
-        <f t="shared" si="11"/>
-        <v>3894.7424712768047</v>
+        <v>3894.1</v>
       </c>
       <c r="F54" s="1">
+        <v>3862.8</v>
+      </c>
+      <c r="G54" s="1">
+        <f>E54-D54</f>
+        <v>64</v>
+      </c>
+      <c r="H54" s="1">
         <f t="shared" si="7"/>
-        <v>3862.8088877768046</v>
-      </c>
-      <c r="G54" s="1">
-        <f t="shared" si="12"/>
-        <v>63.867167000000002</v>
-      </c>
-      <c r="H54" s="1">
+        <v>3.2190000000000003E-2</v>
+      </c>
+      <c r="I54" s="1">
         <f t="shared" si="8"/>
-        <v>3.2190074064806708E-2</v>
-      </c>
-      <c r="I54" s="1">
+        <v>3829.8374400000002</v>
+      </c>
+      <c r="J54" s="1">
         <f t="shared" si="9"/>
-        <v>3829.8462519344425</v>
-      </c>
-      <c r="J54" s="1">
-        <f t="shared" si="13"/>
-        <v>3895.7715236191666</v>
+        <v>3895.7625600000001</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -6180,15 +6181,15 @@
         <v>64.5</v>
       </c>
       <c r="H55" s="1">
+        <f t="shared" si="7"/>
+        <v>3.2555833333333332E-2</v>
+      </c>
+      <c r="I55" s="1">
         <f t="shared" si="8"/>
-        <v>3.2555833333333332E-2</v>
-      </c>
-      <c r="I55" s="1">
+        <v>3873.3628266666665</v>
+      </c>
+      <c r="J55" s="1">
         <f t="shared" si="9"/>
-        <v>3873.3628266666665</v>
-      </c>
-      <c r="J55" s="1">
-        <f t="shared" si="13"/>
         <v>3940.0371733333332</v>
       </c>
       <c r="K55" s="1" t="s">
@@ -6216,19 +6217,19 @@
         <v>3951.6</v>
       </c>
       <c r="G56" s="1">
-        <f t="shared" ref="G56:G61" si="14">E56-D56</f>
+        <f t="shared" ref="G56:G61" si="10">E56-D56</f>
         <v>65.5</v>
       </c>
       <c r="H56" s="1">
+        <f t="shared" si="7"/>
+        <v>3.2930000000000001E-2</v>
+      </c>
+      <c r="I56" s="1">
         <f t="shared" si="8"/>
-        <v>3.2930000000000001E-2</v>
-      </c>
-      <c r="I56" s="1">
+        <v>3917.87968</v>
+      </c>
+      <c r="J56" s="1">
         <f t="shared" si="9"/>
-        <v>3917.87968</v>
-      </c>
-      <c r="J56" s="1">
-        <f t="shared" si="13"/>
         <v>3985.3203199999998</v>
       </c>
       <c r="K56" s="1" t="s">
@@ -6256,19 +6257,19 @@
         <v>3997.6</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>66.199999999999818</v>
       </c>
       <c r="H57" s="1">
+        <f t="shared" si="7"/>
+        <v>3.3313333333333334E-2</v>
+      </c>
+      <c r="I57" s="1">
         <f t="shared" si="8"/>
-        <v>3.3313333333333334E-2</v>
-      </c>
-      <c r="I57" s="1">
+        <v>3963.4871466666664</v>
+      </c>
+      <c r="J57" s="1">
         <f t="shared" si="9"/>
-        <v>3963.4871466666664</v>
-      </c>
-      <c r="J57" s="1">
-        <f t="shared" si="13"/>
         <v>4031.7128533333334</v>
       </c>
       <c r="K57" s="1" t="s">
@@ -6296,19 +6297,19 @@
         <v>4044.7</v>
       </c>
       <c r="G58" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>67</v>
       </c>
       <c r="H58" s="1">
+        <f t="shared" si="7"/>
+        <v>3.3705833333333331E-2</v>
+      </c>
+      <c r="I58" s="1">
         <f t="shared" si="8"/>
-        <v>3.3705833333333331E-2</v>
-      </c>
-      <c r="I58" s="1">
+        <v>4010.1852266666665</v>
+      </c>
+      <c r="J58" s="1">
         <f t="shared" si="9"/>
-        <v>4010.1852266666665</v>
-      </c>
-      <c r="J58" s="1">
-        <f t="shared" si="13"/>
         <v>4079.2147733333331</v>
       </c>
       <c r="K58" s="1" t="s">
@@ -6336,19 +6337,19 @@
         <v>4092.8</v>
       </c>
       <c r="G59" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>67.800000000000182</v>
       </c>
       <c r="H59" s="1">
+        <f t="shared" si="7"/>
+        <v>3.4106666666666667E-2</v>
+      </c>
+      <c r="I59" s="1">
         <f t="shared" si="8"/>
-        <v>3.4106666666666667E-2</v>
-      </c>
-      <c r="I59" s="1">
+        <v>4057.8747733333335</v>
+      </c>
+      <c r="J59" s="1">
         <f t="shared" si="9"/>
-        <v>4057.8747733333335</v>
-      </c>
-      <c r="J59" s="1">
-        <f t="shared" si="13"/>
         <v>4127.7252266666665</v>
       </c>
       <c r="K59" s="1" t="s">
@@ -6376,19 +6377,19 @@
         <v>4142.2</v>
       </c>
       <c r="G60" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>68.600000000000364</v>
       </c>
       <c r="H60" s="1">
+        <f t="shared" si="7"/>
+        <v>3.4518333333333331E-2</v>
+      </c>
+      <c r="I60" s="1">
         <f t="shared" si="8"/>
-        <v>3.4518333333333331E-2</v>
-      </c>
-      <c r="I60" s="1">
+        <v>4106.8532266666662</v>
+      </c>
+      <c r="J60" s="1">
         <f t="shared" si="9"/>
-        <v>4106.8532266666662</v>
-      </c>
-      <c r="J60" s="1">
-        <f t="shared" si="13"/>
         <v>4177.5467733333335</v>
       </c>
       <c r="K60" s="1" t="s">
@@ -6416,19 +6417,19 @@
         <v>4192.7</v>
       </c>
       <c r="G61" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>69.399999999999636</v>
       </c>
       <c r="H61" s="1">
+        <f t="shared" si="7"/>
+        <v>3.4939166666666667E-2</v>
+      </c>
+      <c r="I61" s="1">
         <f t="shared" si="8"/>
-        <v>3.4939166666666667E-2</v>
-      </c>
-      <c r="I61" s="1">
+        <v>4156.9222933333331</v>
+      </c>
+      <c r="J61" s="1">
         <f t="shared" si="9"/>
-        <v>4156.9222933333331</v>
-      </c>
-      <c r="J61" s="1">
-        <f t="shared" si="13"/>
         <v>4228.4777066666666</v>
       </c>
       <c r="K61" s="1" t="s">

</xml_diff>

<commit_message>
Oops, forgot to save the excel sheet.
</commit_message>
<xml_diff>
--- a/OrderInfo.xlsx
+++ b/OrderInfo.xlsx
@@ -253,6 +253,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4111,10 +4112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6434,6 +6435,17 @@
       </c>
       <c r="K61" s="1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>58</v>
+      </c>
+      <c r="B63" s="1">
+        <v>47</v>
+      </c>
+      <c r="C63" s="1">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>